<commit_message>
Push avant dodo ZzzZZzZZzzZZzZzZz
</commit_message>
<xml_diff>
--- a/Equilibrage.xlsx
+++ b/Equilibrage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilisateur\Documents\Github\Dukes Of The Realm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C433F3-DBF0-455A-AA02-AA79F4700FC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB40CB2-8BCB-4C93-AB2D-FCD93B869BDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1033,6 +1033,33 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1048,6 +1075,24 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1057,6 +1102,15 @@
     <xf numFmtId="0" fontId="6" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1084,15 +1138,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1100,15 +1145,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1125,42 +1161,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1605,14 +1605,14 @@
       <c r="F9" s="2"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="74" t="s">
+      <c r="I9" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="J9" s="74"/>
-      <c r="K9" s="74"/>
-      <c r="L9" s="74"/>
-      <c r="M9" s="74"/>
-      <c r="N9" s="74"/>
+      <c r="J9" s="83"/>
+      <c r="K9" s="83"/>
+      <c r="L9" s="83"/>
+      <c r="M9" s="83"/>
+      <c r="N9" s="83"/>
     </row>
     <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
@@ -1632,12 +1632,12 @@
       <c r="G10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="74"/>
-      <c r="J10" s="74"/>
-      <c r="K10" s="74"/>
-      <c r="L10" s="74"/>
-      <c r="M10" s="74"/>
-      <c r="N10" s="74"/>
+      <c r="I10" s="83"/>
+      <c r="J10" s="83"/>
+      <c r="K10" s="83"/>
+      <c r="L10" s="83"/>
+      <c r="M10" s="83"/>
+      <c r="N10" s="83"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
@@ -1667,12 +1667,12 @@
         <f>G3</f>
         <v>65</v>
       </c>
-      <c r="I11" s="74"/>
-      <c r="J11" s="74"/>
-      <c r="K11" s="74"/>
-      <c r="L11" s="74"/>
-      <c r="M11" s="74"/>
-      <c r="N11" s="74"/>
+      <c r="I11" s="83"/>
+      <c r="J11" s="83"/>
+      <c r="K11" s="83"/>
+      <c r="L11" s="83"/>
+      <c r="M11" s="83"/>
+      <c r="N11" s="83"/>
     </row>
     <row r="12" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
@@ -1703,14 +1703,14 @@
         <v>100</v>
       </c>
       <c r="H12" s="1"/>
-      <c r="I12" s="73" t="s">
+      <c r="I12" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="J12" s="73"/>
-      <c r="K12" s="73"/>
-      <c r="L12" s="73"/>
-      <c r="M12" s="73"/>
-      <c r="N12" s="73"/>
+      <c r="J12" s="82"/>
+      <c r="K12" s="82"/>
+      <c r="L12" s="82"/>
+      <c r="M12" s="82"/>
+      <c r="N12" s="82"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
@@ -1741,12 +1741,12 @@
         <v>35</v>
       </c>
       <c r="H13" s="1"/>
-      <c r="I13" s="73"/>
-      <c r="J13" s="73"/>
-      <c r="K13" s="73"/>
-      <c r="L13" s="73"/>
-      <c r="M13" s="73"/>
-      <c r="N13" s="73"/>
+      <c r="I13" s="82"/>
+      <c r="J13" s="82"/>
+      <c r="K13" s="82"/>
+      <c r="L13" s="82"/>
+      <c r="M13" s="82"/>
+      <c r="N13" s="82"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
@@ -1757,12 +1757,12 @@
       <c r="F14" s="2"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="73"/>
-      <c r="J14" s="73"/>
-      <c r="K14" s="73"/>
-      <c r="L14" s="73"/>
-      <c r="M14" s="73"/>
-      <c r="N14" s="73"/>
+      <c r="I14" s="82"/>
+      <c r="J14" s="82"/>
+      <c r="K14" s="82"/>
+      <c r="L14" s="82"/>
+      <c r="M14" s="82"/>
+      <c r="N14" s="82"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
@@ -1771,12 +1771,12 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="73"/>
-      <c r="J15" s="73"/>
-      <c r="K15" s="73"/>
-      <c r="L15" s="73"/>
-      <c r="M15" s="73"/>
-      <c r="N15" s="73"/>
+      <c r="I15" s="82"/>
+      <c r="J15" s="82"/>
+      <c r="K15" s="82"/>
+      <c r="L15" s="82"/>
+      <c r="M15" s="82"/>
+      <c r="N15" s="82"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
@@ -3169,242 +3169,237 @@
   <sheetData>
     <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="105"/>
-      <c r="D3" s="105"/>
-      <c r="E3" s="105"/>
-      <c r="F3" s="106"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="89"/>
       <c r="G3" s="21"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="96" t="s">
+      <c r="B4" s="90" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="97"/>
-      <c r="D4" s="97"/>
-      <c r="E4" s="98"/>
+      <c r="C4" s="91"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="92"/>
       <c r="F4" s="29">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="84" t="s">
+      <c r="B5" s="102" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="85"/>
-      <c r="D5" s="85"/>
-      <c r="E5" s="86"/>
+      <c r="C5" s="103"/>
+      <c r="D5" s="103"/>
+      <c r="E5" s="104"/>
       <c r="F5" s="35">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="78" t="s">
+      <c r="B6" s="93" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="79"/>
-      <c r="D6" s="79"/>
-      <c r="E6" s="80"/>
+      <c r="C6" s="94"/>
+      <c r="D6" s="94"/>
+      <c r="E6" s="95"/>
       <c r="F6" s="27">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="90" t="s">
+      <c r="B7" s="96" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="91"/>
-      <c r="D7" s="91"/>
-      <c r="E7" s="92"/>
+      <c r="C7" s="97"/>
+      <c r="D7" s="97"/>
+      <c r="E7" s="98"/>
       <c r="F7" s="22">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="78" t="s">
+      <c r="B8" s="93" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="79"/>
-      <c r="D8" s="79"/>
-      <c r="E8" s="80"/>
+      <c r="C8" s="94"/>
+      <c r="D8" s="94"/>
+      <c r="E8" s="95"/>
       <c r="F8" s="27">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="102" t="s">
+      <c r="B9" s="114" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="91"/>
-      <c r="D9" s="91"/>
-      <c r="E9" s="92"/>
+      <c r="C9" s="97"/>
+      <c r="D9" s="97"/>
+      <c r="E9" s="98"/>
       <c r="F9" s="22">
         <v>250</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="93" t="s">
+      <c r="B10" s="108" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="94"/>
-      <c r="D10" s="94"/>
-      <c r="E10" s="95"/>
+      <c r="C10" s="109"/>
+      <c r="D10" s="109"/>
+      <c r="E10" s="110"/>
       <c r="F10" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="103" t="s">
+      <c r="B11" s="115" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="82"/>
-      <c r="D11" s="82"/>
-      <c r="E11" s="83"/>
+      <c r="C11" s="100"/>
+      <c r="D11" s="100"/>
+      <c r="E11" s="101"/>
       <c r="F11" s="28">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="96" t="s">
+      <c r="B12" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="97"/>
-      <c r="D12" s="97"/>
-      <c r="E12" s="98"/>
+      <c r="C12" s="91"/>
+      <c r="D12" s="91"/>
+      <c r="E12" s="92"/>
       <c r="F12" s="29">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="75" t="s">
+      <c r="B13" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="76"/>
-      <c r="D13" s="76"/>
-      <c r="E13" s="77"/>
+      <c r="C13" s="85"/>
+      <c r="D13" s="85"/>
+      <c r="E13" s="86"/>
       <c r="F13" s="23">
         <v>10</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="78" t="s">
+      <c r="B14" s="93" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="79"/>
-      <c r="D14" s="79"/>
-      <c r="E14" s="80"/>
+      <c r="C14" s="94"/>
+      <c r="D14" s="94"/>
+      <c r="E14" s="95"/>
       <c r="F14" s="24">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="90" t="s">
+      <c r="B15" s="96" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="91"/>
-      <c r="D15" s="91"/>
-      <c r="E15" s="92"/>
+      <c r="C15" s="97"/>
+      <c r="D15" s="97"/>
+      <c r="E15" s="98"/>
       <c r="F15" s="31">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="93" t="s">
+      <c r="B16" s="108" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="94"/>
-      <c r="D16" s="94"/>
-      <c r="E16" s="95"/>
+      <c r="C16" s="109"/>
+      <c r="D16" s="109"/>
+      <c r="E16" s="110"/>
       <c r="F16" s="25">
         <v>20</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="81" t="s">
+      <c r="B17" s="99" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="82"/>
-      <c r="D17" s="82"/>
-      <c r="E17" s="83"/>
+      <c r="C17" s="100"/>
+      <c r="D17" s="100"/>
+      <c r="E17" s="101"/>
       <c r="F17" s="32">
         <v>0.9</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="96" t="s">
+      <c r="B18" s="90" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="97"/>
-      <c r="D18" s="97"/>
-      <c r="E18" s="98"/>
+      <c r="C18" s="91"/>
+      <c r="D18" s="91"/>
+      <c r="E18" s="92"/>
       <c r="F18" s="33">
         <v>3</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="81" t="s">
+      <c r="B19" s="99" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="82"/>
-      <c r="D19" s="82"/>
-      <c r="E19" s="83"/>
+      <c r="C19" s="100"/>
+      <c r="D19" s="100"/>
+      <c r="E19" s="101"/>
       <c r="F19" s="34">
         <v>0.66700000000000004</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="99" t="s">
+      <c r="B20" s="111" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="100"/>
-      <c r="D20" s="100"/>
-      <c r="E20" s="101"/>
+      <c r="C20" s="112"/>
+      <c r="D20" s="112"/>
+      <c r="E20" s="113"/>
       <c r="F20" s="30">
         <v>12</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="75" t="s">
+      <c r="B21" s="84" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="76"/>
-      <c r="D21" s="76"/>
-      <c r="E21" s="77"/>
+      <c r="C21" s="85"/>
+      <c r="D21" s="85"/>
+      <c r="E21" s="86"/>
       <c r="F21" s="23">
         <v>3</v>
       </c>
     </row>
     <row r="22" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="78" t="s">
+      <c r="B22" s="93" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="79"/>
-      <c r="D22" s="79"/>
-      <c r="E22" s="80"/>
+      <c r="C22" s="94"/>
+      <c r="D22" s="94"/>
+      <c r="E22" s="95"/>
       <c r="F22" s="24">
         <v>4</v>
       </c>
     </row>
     <row r="23" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="87" t="s">
+      <c r="B23" s="105" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="88"/>
-      <c r="D23" s="88"/>
-      <c r="E23" s="89"/>
+      <c r="C23" s="106"/>
+      <c r="D23" s="106"/>
+      <c r="E23" s="107"/>
       <c r="F23" s="36">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
     <mergeCell ref="B21:E21"/>
     <mergeCell ref="B22:E22"/>
     <mergeCell ref="B19:E19"/>
@@ -3421,6 +3416,11 @@
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3429,10 +3429,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7358574A-592A-4C40-9736-421EE2E19A0C}">
-  <dimension ref="A2:X27"/>
+  <dimension ref="A2:X28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="X5" sqref="X5"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3450,19 +3450,19 @@
       <c r="S2" t="s">
         <v>61</v>
       </c>
-      <c r="T2" s="113">
+      <c r="T2" s="79">
         <v>0</v>
       </c>
-      <c r="U2" s="113">
+      <c r="U2" s="79">
         <v>1</v>
       </c>
-      <c r="V2" s="113">
+      <c r="V2" s="79">
         <v>1</v>
       </c>
-      <c r="W2" s="113">
+      <c r="W2" s="79">
         <v>3</v>
       </c>
-      <c r="X2" s="113">
+      <c r="X2" s="79">
         <v>6</v>
       </c>
     </row>
@@ -3491,37 +3491,37 @@
       <c r="L3" t="s">
         <v>63</v>
       </c>
-      <c r="M3" s="113">
+      <c r="M3" s="79">
         <v>200</v>
       </c>
-      <c r="N3" s="113">
+      <c r="N3" s="79">
         <v>300</v>
       </c>
-      <c r="O3" s="113">
+      <c r="O3" s="79">
         <v>250</v>
       </c>
-      <c r="P3" s="113">
+      <c r="P3" s="79">
         <v>100</v>
       </c>
-      <c r="Q3" s="113">
+      <c r="Q3" s="79">
         <v>200</v>
       </c>
       <c r="S3" t="s">
         <v>62</v>
       </c>
-      <c r="T3" s="113">
+      <c r="T3" s="79">
         <v>4</v>
       </c>
-      <c r="U3" s="113">
+      <c r="U3" s="79">
         <v>3</v>
       </c>
-      <c r="V3" s="113">
+      <c r="V3" s="79">
         <v>3</v>
       </c>
-      <c r="W3" s="113">
+      <c r="W3" s="79">
         <v>2</v>
       </c>
-      <c r="X3" s="113">
+      <c r="X3" s="79">
         <v>5</v>
       </c>
     </row>
@@ -3554,40 +3554,40 @@
       <c r="J4" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="L4" s="107" t="s">
+      <c r="L4" s="73" t="s">
         <v>48</v>
       </c>
-      <c r="M4" s="107" t="s">
+      <c r="M4" s="73" t="s">
         <v>49</v>
       </c>
-      <c r="N4" s="107" t="s">
+      <c r="N4" s="73" t="s">
         <v>50</v>
       </c>
-      <c r="O4" s="115" t="s">
+      <c r="O4" s="81" t="s">
         <v>55</v>
       </c>
-      <c r="P4" s="107" t="s">
+      <c r="P4" s="73" t="s">
         <v>58</v>
       </c>
-      <c r="Q4" s="107" t="s">
+      <c r="Q4" s="73" t="s">
         <v>47</v>
       </c>
-      <c r="S4" s="107" t="s">
+      <c r="S4" s="73" t="s">
         <v>48</v>
       </c>
-      <c r="T4" s="107" t="s">
+      <c r="T4" s="73" t="s">
         <v>49</v>
       </c>
-      <c r="U4" s="107" t="s">
+      <c r="U4" s="73" t="s">
         <v>50</v>
       </c>
-      <c r="V4" s="107" t="s">
+      <c r="V4" s="73" t="s">
         <v>55</v>
       </c>
-      <c r="W4" s="107" t="s">
+      <c r="W4" s="73" t="s">
         <v>58</v>
       </c>
-      <c r="X4" s="107" t="s">
+      <c r="X4" s="73" t="s">
         <v>47</v>
       </c>
     </row>
@@ -3610,15 +3610,15 @@
         <v>3</v>
       </c>
       <c r="J5" s="1">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="L5" s="1">
         <v>0</v>
       </c>
       <c r="M5" s="69"/>
       <c r="N5" s="69"/>
-      <c r="O5" s="109"/>
-      <c r="P5" s="110">
+      <c r="O5" s="75"/>
+      <c r="P5" s="76">
         <f>100 + L6*L6*L6*L6 / 4</f>
         <v>100.25</v>
       </c>
@@ -3631,8 +3631,8 @@
       </c>
       <c r="T5" s="69"/>
       <c r="U5" s="69"/>
-      <c r="V5" s="109"/>
-      <c r="W5" s="110">
+      <c r="V5" s="75"/>
+      <c r="W5" s="76">
         <v>3</v>
       </c>
       <c r="X5" s="48">
@@ -3651,8 +3651,8 @@
         <v>1</v>
       </c>
       <c r="D6" s="48">
-        <f>$J$11+A6*EXP(A6/10)</f>
-        <v>71.105170918075643</v>
+        <f>80+6*A6</f>
+        <v>86</v>
       </c>
       <c r="E6" s="48">
         <f>$E$2+A6*$E$2+EXP(A6/4)</f>
@@ -3679,19 +3679,19 @@
       <c r="L6" s="1">
         <v>1</v>
       </c>
-      <c r="M6" s="111">
+      <c r="M6" s="77">
         <f>200*L8+L8*L8*L8*L8/7</f>
         <v>611.57142857142856</v>
       </c>
-      <c r="N6" s="108">
+      <c r="N6" s="74">
         <f>300*L6+L6*L7*L8</f>
         <v>306</v>
       </c>
-      <c r="O6" s="114">
+      <c r="O6" s="80">
         <f>250*L6+L6*L6*L6</f>
         <v>251</v>
       </c>
-      <c r="P6" s="110">
+      <c r="P6" s="76">
         <f t="shared" ref="P6:P15" si="0">100 + L7*L7*L7*L7 / 4</f>
         <v>104</v>
       </c>
@@ -3699,19 +3699,23 @@
         <f t="shared" ref="Q6:Q25" si="1">200*L7 + L6*L6*(L6/2)</f>
         <v>400.5</v>
       </c>
+      <c r="R6" s="64">
+        <f>V6*G6/100</f>
+        <v>3.9127455834853744</v>
+      </c>
       <c r="S6" s="1">
         <v>1</v>
       </c>
-      <c r="T6" s="111">
+      <c r="T6" s="77">
         <v>4</v>
       </c>
-      <c r="U6" s="108">
+      <c r="U6" s="74">
         <v>4</v>
       </c>
-      <c r="V6" s="112">
+      <c r="V6" s="78">
         <v>4</v>
       </c>
-      <c r="W6" s="110">
+      <c r="W6" s="76">
         <v>5</v>
       </c>
       <c r="X6" s="48">
@@ -3730,23 +3734,23 @@
         <v>1</v>
       </c>
       <c r="D7" s="48">
-        <f>$J$11+A7*EXP(A7/10)</f>
-        <v>72.442805516320334</v>
+        <f t="shared" ref="D7:D25" si="2">80+6*A7</f>
+        <v>92</v>
       </c>
       <c r="E7" s="48">
-        <f t="shared" ref="E7:E25" si="2">$E$2+A7*$E$2+EXP(A7/4)</f>
+        <f t="shared" ref="E7:E25" si="3">$E$2+A7*$E$2+EXP(A7/4)</f>
         <v>16.648721270700129</v>
       </c>
       <c r="F7" s="48">
-        <f t="shared" ref="F7:F25" si="3">E7*60</f>
+        <f t="shared" ref="F7:F25" si="4">E7*60</f>
         <v>998.92327624200777</v>
       </c>
       <c r="G7" s="48">
-        <f t="shared" ref="G7:G25" si="4">100-EXP(A7/6)-A7</f>
+        <f t="shared" ref="G7:G25" si="5">100-EXP(A7/6)-A7</f>
         <v>96.604387574913915</v>
       </c>
       <c r="H7" s="48">
-        <f t="shared" ref="H7:H15" si="5">A7*(A7/2)+A7</f>
+        <f t="shared" ref="H7:H15" si="6">A7*(A7/2)+A7</f>
         <v>4</v>
       </c>
       <c r="I7" s="1" t="s">
@@ -3758,19 +3762,19 @@
       <c r="L7" s="1">
         <v>2</v>
       </c>
-      <c r="M7" s="111">
-        <f t="shared" ref="M7:M15" si="6">200*L9+L9*L9*L9*L9/7</f>
+      <c r="M7" s="77">
+        <f t="shared" ref="M7:M15" si="7">200*L9+L9*L9*L9*L9/7</f>
         <v>836.57142857142856</v>
       </c>
-      <c r="N7" s="108">
-        <f t="shared" ref="N7:N25" si="7">300*L7+L7*L8*L9</f>
+      <c r="N7" s="74">
+        <f t="shared" ref="N7:N25" si="8">300*L7+L7*L8*L9</f>
         <v>624</v>
       </c>
-      <c r="O7" s="114">
-        <f t="shared" ref="O7:O25" si="8">250*L7+L7*L7*L7</f>
+      <c r="O7" s="80">
+        <f t="shared" ref="O7:O25" si="9">250*L7+L7*L7*L7</f>
         <v>508</v>
       </c>
-      <c r="P7" s="110">
+      <c r="P7" s="76">
         <f t="shared" si="0"/>
         <v>120.25</v>
       </c>
@@ -3778,19 +3782,23 @@
         <f t="shared" si="1"/>
         <v>604</v>
       </c>
+      <c r="R7" s="64">
+        <f t="shared" ref="R7:R25" si="10">V7*G7/100</f>
+        <v>6.7623071302439737</v>
+      </c>
       <c r="S7" s="1">
         <v>2</v>
       </c>
-      <c r="T7" s="111">
+      <c r="T7" s="77">
         <v>8</v>
       </c>
-      <c r="U7" s="108">
+      <c r="U7" s="74">
         <v>7</v>
       </c>
-      <c r="V7" s="112">
+      <c r="V7" s="78">
         <v>7</v>
       </c>
-      <c r="W7" s="110">
+      <c r="W7" s="76">
         <v>7</v>
       </c>
       <c r="X7" s="48">
@@ -3802,30 +3810,30 @@
         <v>3</v>
       </c>
       <c r="B8" s="49">
-        <f t="shared" ref="B8:B15" si="9">B7+0.05</f>
+        <f t="shared" ref="B8:B15" si="11">B7+0.05</f>
         <v>1.1500000000000001</v>
       </c>
       <c r="C8" s="65">
         <v>2</v>
       </c>
       <c r="D8" s="48">
-        <f>$J$11+A8*EXP(A8/10)</f>
-        <v>74.049576422728009</v>
+        <f t="shared" si="2"/>
+        <v>98</v>
       </c>
       <c r="E8" s="48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>22.117000016612675</v>
       </c>
       <c r="F8" s="48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1327.0200009967605</v>
       </c>
       <c r="G8" s="48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>95.351278729299878</v>
       </c>
       <c r="H8" s="48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7.5</v>
       </c>
       <c r="I8" s="1" t="s">
@@ -3837,19 +3845,19 @@
       <c r="L8" s="1">
         <v>3</v>
       </c>
-      <c r="M8" s="111">
-        <f t="shared" si="6"/>
+      <c r="M8" s="77">
+        <f t="shared" si="7"/>
         <v>1089.2857142857142</v>
       </c>
-      <c r="N8" s="108">
-        <f t="shared" si="7"/>
+      <c r="N8" s="74">
+        <f t="shared" si="8"/>
         <v>960</v>
       </c>
-      <c r="O8" s="114">
-        <f t="shared" si="8"/>
+      <c r="O8" s="80">
+        <f t="shared" si="9"/>
         <v>777</v>
       </c>
-      <c r="P8" s="110">
+      <c r="P8" s="76">
         <f t="shared" si="0"/>
         <v>164</v>
       </c>
@@ -3857,19 +3865,23 @@
         <f t="shared" si="1"/>
         <v>813.5</v>
       </c>
+      <c r="R8" s="64">
+        <f t="shared" si="10"/>
+        <v>9.5351278729299889</v>
+      </c>
       <c r="S8" s="1">
         <v>3</v>
       </c>
-      <c r="T8" s="111">
+      <c r="T8" s="77">
         <v>12</v>
       </c>
-      <c r="U8" s="108">
+      <c r="U8" s="74">
         <v>10</v>
       </c>
-      <c r="V8" s="112">
+      <c r="V8" s="78">
         <v>10</v>
       </c>
-      <c r="W8" s="110">
+      <c r="W8" s="76">
         <v>9</v>
       </c>
       <c r="X8" s="48">
@@ -3881,30 +3893,30 @@
         <v>4</v>
       </c>
       <c r="B9" s="49">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1.2000000000000002</v>
       </c>
       <c r="C9" s="65">
         <v>2</v>
       </c>
       <c r="D9" s="48">
-        <f>$J$11+A9*EXP(A9/10)</f>
-        <v>75.967298790565081</v>
+        <f t="shared" si="2"/>
+        <v>104</v>
       </c>
       <c r="E9" s="48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>27.718281828459045</v>
       </c>
       <c r="F9" s="48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1663.0969097075426</v>
       </c>
       <c r="G9" s="48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>94.052265958945327</v>
       </c>
       <c r="H9" s="48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="I9" s="1" t="s">
@@ -3916,19 +3928,19 @@
       <c r="L9" s="1">
         <v>4</v>
       </c>
-      <c r="M9" s="111">
-        <f t="shared" si="6"/>
+      <c r="M9" s="77">
+        <f t="shared" si="7"/>
         <v>1385.1428571428571</v>
       </c>
-      <c r="N9" s="108">
-        <f t="shared" si="7"/>
+      <c r="N9" s="74">
+        <f t="shared" si="8"/>
         <v>1320</v>
       </c>
-      <c r="O9" s="114">
-        <f t="shared" si="8"/>
+      <c r="O9" s="80">
+        <f t="shared" si="9"/>
         <v>1064</v>
       </c>
-      <c r="P9" s="110">
+      <c r="P9" s="76">
         <f t="shared" si="0"/>
         <v>256.25</v>
       </c>
@@ -3936,19 +3948,23 @@
         <f t="shared" si="1"/>
         <v>1032</v>
       </c>
+      <c r="R9" s="64">
+        <f t="shared" si="10"/>
+        <v>12.226794574662893</v>
+      </c>
       <c r="S9" s="1">
         <v>4</v>
       </c>
-      <c r="T9" s="111">
+      <c r="T9" s="77">
         <v>16</v>
       </c>
-      <c r="U9" s="108">
+      <c r="U9" s="74">
         <v>13</v>
       </c>
-      <c r="V9" s="112">
+      <c r="V9" s="78">
         <v>13</v>
       </c>
-      <c r="W9" s="110">
+      <c r="W9" s="76">
         <v>11</v>
       </c>
       <c r="X9" s="48">
@@ -3960,30 +3976,30 @@
         <v>5</v>
       </c>
       <c r="B10" s="49">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1.2500000000000002</v>
       </c>
       <c r="C10" s="65">
         <v>3</v>
       </c>
       <c r="D10" s="48">
-        <f>$J$11+A10*EXP(A10/10)</f>
-        <v>78.243606353500638</v>
+        <f t="shared" si="2"/>
+        <v>110</v>
       </c>
       <c r="E10" s="48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>33.490342957461841</v>
       </c>
       <c r="F10" s="48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2009.4205774477105</v>
       </c>
       <c r="G10" s="48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>92.699024109107171</v>
       </c>
       <c r="H10" s="48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>17.5</v>
       </c>
       <c r="I10" s="1" t="s">
@@ -3995,19 +4011,19 @@
       <c r="L10" s="1">
         <v>5</v>
       </c>
-      <c r="M10" s="111">
-        <f t="shared" si="6"/>
+      <c r="M10" s="77">
+        <f t="shared" si="7"/>
         <v>1743</v>
       </c>
-      <c r="N10" s="108">
-        <f t="shared" si="7"/>
+      <c r="N10" s="74">
+        <f t="shared" si="8"/>
         <v>1710</v>
       </c>
-      <c r="O10" s="114">
-        <f t="shared" si="8"/>
+      <c r="O10" s="80">
+        <f t="shared" si="9"/>
         <v>1375</v>
       </c>
-      <c r="P10" s="110">
+      <c r="P10" s="76">
         <f t="shared" si="0"/>
         <v>424</v>
       </c>
@@ -4015,19 +4031,23 @@
         <f t="shared" si="1"/>
         <v>1262.5</v>
       </c>
+      <c r="R10" s="64">
+        <f t="shared" si="10"/>
+        <v>14.831843857457148</v>
+      </c>
       <c r="S10" s="1">
         <v>5</v>
       </c>
-      <c r="T10" s="111">
+      <c r="T10" s="77">
         <v>20</v>
       </c>
-      <c r="U10" s="108">
+      <c r="U10" s="74">
         <v>16</v>
       </c>
-      <c r="V10" s="112">
+      <c r="V10" s="78">
         <v>16</v>
       </c>
-      <c r="W10" s="110">
+      <c r="W10" s="76">
         <v>13</v>
       </c>
       <c r="X10" s="48">
@@ -4039,53 +4059,53 @@
         <v>6</v>
       </c>
       <c r="B11" s="49">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1.3000000000000003</v>
       </c>
       <c r="C11" s="65">
         <v>3</v>
       </c>
       <c r="D11" s="48">
-        <f>$J$11+A11*EXP(A11/10)</f>
-        <v>80.932712802343048</v>
+        <f t="shared" si="2"/>
+        <v>116</v>
       </c>
       <c r="E11" s="48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>39.481689070338064</v>
       </c>
       <c r="F11" s="48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2368.901344220284</v>
       </c>
       <c r="G11" s="48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>91.281718171540959</v>
       </c>
       <c r="H11" s="48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>24</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1">
-        <f>J5+J6*2+J8+J7*3+J9+J10*2</f>
-        <v>70</v>
+        <f>J5+J6*2+J7*3+J8+J9+J10*2</f>
+        <v>67</v>
       </c>
       <c r="L11" s="1">
         <v>6</v>
       </c>
-      <c r="M11" s="111">
-        <f t="shared" si="6"/>
+      <c r="M11" s="77">
+        <f t="shared" si="7"/>
         <v>2185.1428571428569</v>
       </c>
-      <c r="N11" s="108">
-        <f t="shared" si="7"/>
+      <c r="N11" s="74">
+        <f t="shared" si="8"/>
         <v>2136</v>
       </c>
-      <c r="O11" s="114">
-        <f t="shared" si="8"/>
+      <c r="O11" s="80">
+        <f t="shared" si="9"/>
         <v>1716</v>
       </c>
-      <c r="P11" s="110">
+      <c r="P11" s="76">
         <f t="shared" si="0"/>
         <v>700.25</v>
       </c>
@@ -4093,19 +4113,23 @@
         <f t="shared" si="1"/>
         <v>1508</v>
       </c>
+      <c r="R11" s="64">
+        <f t="shared" si="10"/>
+        <v>17.343526452592783</v>
+      </c>
       <c r="S11" s="1">
         <v>6</v>
       </c>
-      <c r="T11" s="111">
+      <c r="T11" s="77">
         <v>24</v>
       </c>
-      <c r="U11" s="108">
+      <c r="U11" s="74">
         <v>19</v>
       </c>
-      <c r="V11" s="112">
+      <c r="V11" s="78">
         <v>19</v>
       </c>
-      <c r="W11" s="110">
+      <c r="W11" s="76">
         <v>15</v>
       </c>
       <c r="X11" s="48">
@@ -4117,48 +4141,48 @@
         <v>7</v>
       </c>
       <c r="B12" s="49">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1.3500000000000003</v>
       </c>
       <c r="C12" s="65">
         <v>4</v>
       </c>
       <c r="D12" s="48">
-        <f>$J$11+A12*EXP(A12/10)</f>
-        <v>84.096268952293343</v>
+        <f t="shared" si="2"/>
+        <v>122</v>
       </c>
       <c r="E12" s="48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>45.754602676005732</v>
       </c>
       <c r="F12" s="48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2745.2761605603437</v>
       </c>
       <c r="G12" s="48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>89.78872945684644</v>
       </c>
       <c r="H12" s="48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>31.5</v>
       </c>
       <c r="L12" s="1">
         <v>7</v>
       </c>
-      <c r="M12" s="111">
-        <f t="shared" si="6"/>
+      <c r="M12" s="77">
+        <f t="shared" si="7"/>
         <v>2737.2857142857142</v>
       </c>
-      <c r="N12" s="108">
-        <f t="shared" si="7"/>
+      <c r="N12" s="74">
+        <f t="shared" si="8"/>
         <v>2604</v>
       </c>
-      <c r="O12" s="114">
-        <f t="shared" si="8"/>
+      <c r="O12" s="80">
+        <f t="shared" si="9"/>
         <v>2093</v>
       </c>
-      <c r="P12" s="110">
+      <c r="P12" s="76">
         <f t="shared" si="0"/>
         <v>1124</v>
       </c>
@@ -4166,19 +4190,23 @@
         <f t="shared" si="1"/>
         <v>1771.5</v>
       </c>
+      <c r="R12" s="64">
+        <f t="shared" si="10"/>
+        <v>19.753520480506218</v>
+      </c>
       <c r="S12" s="1">
         <v>7</v>
       </c>
-      <c r="T12" s="111">
+      <c r="T12" s="77">
         <v>28</v>
       </c>
-      <c r="U12" s="108">
+      <c r="U12" s="74">
         <v>22</v>
       </c>
-      <c r="V12" s="112">
+      <c r="V12" s="78">
         <v>22</v>
       </c>
-      <c r="W12" s="110">
+      <c r="W12" s="76">
         <v>17</v>
       </c>
       <c r="X12" s="48">
@@ -4190,30 +4218,30 @@
         <v>8</v>
       </c>
       <c r="B13" s="49">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1.4000000000000004</v>
       </c>
       <c r="C13" s="65">
         <v>4</v>
       </c>
       <c r="D13" s="48">
-        <f>$J$11+A13*EXP(A13/10)</f>
-        <v>87.804327427939739</v>
+        <f t="shared" si="2"/>
+        <v>128</v>
       </c>
       <c r="E13" s="48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>52.389056098930652</v>
       </c>
       <c r="F13" s="48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3143.3433659358393</v>
       </c>
       <c r="G13" s="48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>88.206332105316818</v>
       </c>
       <c r="H13" s="48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>40</v>
       </c>
       <c r="I13" s="1"/>
@@ -4221,19 +4249,19 @@
       <c r="L13" s="1">
         <v>8</v>
       </c>
-      <c r="M13" s="111">
-        <f t="shared" si="6"/>
+      <c r="M13" s="77">
+        <f t="shared" si="7"/>
         <v>3428.5714285714284</v>
       </c>
-      <c r="N13" s="108">
-        <f t="shared" si="7"/>
+      <c r="N13" s="74">
+        <f t="shared" si="8"/>
         <v>3120</v>
       </c>
-      <c r="O13" s="114">
-        <f t="shared" si="8"/>
+      <c r="O13" s="80">
+        <f t="shared" si="9"/>
         <v>2512</v>
       </c>
-      <c r="P13" s="110">
+      <c r="P13" s="76">
         <f t="shared" si="0"/>
         <v>1740.25</v>
       </c>
@@ -4241,19 +4269,23 @@
         <f t="shared" si="1"/>
         <v>2056</v>
       </c>
+      <c r="R13" s="64">
+        <f t="shared" si="10"/>
+        <v>22.051583026329205</v>
+      </c>
       <c r="S13" s="1">
         <v>8</v>
       </c>
-      <c r="T13" s="111">
+      <c r="T13" s="77">
         <v>32</v>
       </c>
-      <c r="U13" s="108">
+      <c r="U13" s="74">
         <v>25</v>
       </c>
-      <c r="V13" s="112">
+      <c r="V13" s="78">
         <v>25</v>
       </c>
-      <c r="W13" s="110">
+      <c r="W13" s="76">
         <v>19</v>
       </c>
       <c r="X13" s="48">
@@ -4265,30 +4297,30 @@
         <v>9</v>
       </c>
       <c r="B14" s="49">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1.4500000000000004</v>
       </c>
       <c r="C14" s="65">
         <v>5</v>
       </c>
       <c r="D14" s="48">
-        <f>$J$11+A14*EXP(A14/10)</f>
-        <v>92.13642800041255</v>
+        <f t="shared" si="2"/>
+        <v>134</v>
       </c>
       <c r="E14" s="48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>59.487735836358524</v>
       </c>
       <c r="F14" s="48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3569.2641501815115</v>
       </c>
       <c r="G14" s="48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>86.518310929661936</v>
       </c>
       <c r="H14" s="48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>49.5</v>
       </c>
       <c r="I14" s="1"/>
@@ -4296,19 +4328,19 @@
       <c r="L14" s="1">
         <v>9</v>
       </c>
-      <c r="M14" s="111">
-        <f t="shared" si="6"/>
+      <c r="M14" s="77">
+        <f t="shared" si="7"/>
         <v>4291.5714285714284</v>
       </c>
-      <c r="N14" s="108">
-        <f t="shared" si="7"/>
+      <c r="N14" s="74">
+        <f t="shared" si="8"/>
         <v>3690</v>
       </c>
-      <c r="O14" s="114">
-        <f t="shared" si="8"/>
+      <c r="O14" s="80">
+        <f t="shared" si="9"/>
         <v>2979</v>
       </c>
-      <c r="P14" s="110">
+      <c r="P14" s="76">
         <f t="shared" si="0"/>
         <v>2600</v>
       </c>
@@ -4316,19 +4348,23 @@
         <f t="shared" si="1"/>
         <v>2364.5</v>
       </c>
+      <c r="R14" s="64">
+        <f t="shared" si="10"/>
+        <v>24.22512706030534</v>
+      </c>
       <c r="S14" s="1">
         <v>9</v>
       </c>
-      <c r="T14" s="111">
+      <c r="T14" s="77">
         <v>36</v>
       </c>
-      <c r="U14" s="108">
+      <c r="U14" s="74">
         <v>28</v>
       </c>
-      <c r="V14" s="112">
+      <c r="V14" s="78">
         <v>28</v>
       </c>
-      <c r="W14" s="110">
+      <c r="W14" s="76">
         <v>21</v>
       </c>
       <c r="X14" s="48">
@@ -4340,30 +4376,30 @@
         <v>10</v>
       </c>
       <c r="B15" s="49">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1.5000000000000004</v>
       </c>
       <c r="C15" s="65">
         <v>6</v>
       </c>
       <c r="D15" s="48">
-        <f>$J$11+A15*EXP(A15/10)</f>
-        <v>97.182818284590454</v>
+        <f t="shared" si="2"/>
+        <v>140</v>
       </c>
       <c r="E15" s="48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>67.182493960703468</v>
       </c>
       <c r="F15" s="48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4030.949637642208</v>
       </c>
       <c r="G15" s="48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>84.705509949529969</v>
       </c>
       <c r="H15" s="48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>60</v>
       </c>
       <c r="I15" s="1"/>
@@ -4371,19 +4407,19 @@
       <c r="L15" s="1">
         <v>10</v>
       </c>
-      <c r="M15" s="111">
-        <f t="shared" si="6"/>
+      <c r="M15" s="77">
+        <f t="shared" si="7"/>
         <v>5362.2857142857138</v>
       </c>
-      <c r="N15" s="108">
-        <f t="shared" si="7"/>
+      <c r="N15" s="74">
+        <f t="shared" si="8"/>
         <v>4320</v>
       </c>
-      <c r="O15" s="114">
-        <f t="shared" si="8"/>
+      <c r="O15" s="80">
+        <f t="shared" si="9"/>
         <v>3500</v>
       </c>
-      <c r="P15" s="110">
+      <c r="P15" s="76">
         <f t="shared" si="0"/>
         <v>3760.25</v>
       </c>
@@ -4391,19 +4427,23 @@
         <f t="shared" si="1"/>
         <v>2700</v>
       </c>
+      <c r="R15" s="64">
+        <f t="shared" si="10"/>
+        <v>26.258708084354289</v>
+      </c>
       <c r="S15" s="1">
         <v>10</v>
       </c>
-      <c r="T15" s="111">
+      <c r="T15" s="77">
         <v>40</v>
       </c>
-      <c r="U15" s="108">
+      <c r="U15" s="74">
         <v>31</v>
       </c>
-      <c r="V15" s="112">
+      <c r="V15" s="78">
         <v>31</v>
       </c>
-      <c r="W15" s="110">
+      <c r="W15" s="76">
         <v>23</v>
       </c>
       <c r="X15" s="48">
@@ -4420,19 +4460,19 @@
       </c>
       <c r="C16" s="68"/>
       <c r="D16" s="48">
-        <f>$J$11+A16*EXP(A16/10)</f>
-        <v>103.04582626341076</v>
+        <f t="shared" si="2"/>
+        <v>146</v>
       </c>
       <c r="E16" s="48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>75.642631884188177</v>
       </c>
       <c r="F16" s="48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4538.5579130512906</v>
       </c>
       <c r="G16" s="48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>82.745299048063671</v>
       </c>
       <c r="I16" s="1"/>
@@ -4441,12 +4481,12 @@
         <v>11</v>
       </c>
       <c r="M16" s="1"/>
-      <c r="N16" s="108">
-        <f t="shared" si="7"/>
+      <c r="N16" s="74">
+        <f t="shared" si="8"/>
         <v>5016</v>
       </c>
-      <c r="O16" s="114">
-        <f t="shared" si="8"/>
+      <c r="O16" s="80">
+        <f t="shared" si="9"/>
         <v>4081</v>
       </c>
       <c r="P16" s="1"/>
@@ -4454,14 +4494,18 @@
         <f t="shared" si="1"/>
         <v>3065.5</v>
       </c>
+      <c r="R16" s="64">
+        <f t="shared" si="10"/>
+        <v>28.133401676341649</v>
+      </c>
       <c r="S16" s="1">
         <v>11</v>
       </c>
       <c r="T16" s="1"/>
-      <c r="U16" s="108">
+      <c r="U16" s="74">
         <v>34</v>
       </c>
-      <c r="V16" s="112">
+      <c r="V16" s="78">
         <v>34</v>
       </c>
       <c r="W16" s="1"/>
@@ -4479,19 +4523,19 @@
       </c>
       <c r="C17" s="68"/>
       <c r="D17" s="48">
-        <f>$J$11+A17*EXP(A17/10)</f>
-        <v>109.84140307283857</v>
+        <f t="shared" si="2"/>
+        <v>152</v>
       </c>
       <c r="E17" s="48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>85.085536923187675</v>
       </c>
       <c r="F17" s="48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5105.1322153912606</v>
       </c>
       <c r="G17" s="48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>80.610943901069348</v>
       </c>
       <c r="I17" s="1"/>
@@ -4500,12 +4544,12 @@
         <v>12</v>
       </c>
       <c r="M17" s="1"/>
-      <c r="N17" s="108">
-        <f t="shared" si="7"/>
+      <c r="N17" s="74">
+        <f t="shared" si="8"/>
         <v>5784</v>
       </c>
-      <c r="O17" s="114">
-        <f t="shared" si="8"/>
+      <c r="O17" s="80">
+        <f t="shared" si="9"/>
         <v>4728</v>
       </c>
       <c r="P17" s="1"/>
@@ -4513,14 +4557,18 @@
         <f t="shared" si="1"/>
         <v>3464</v>
       </c>
+      <c r="R17" s="64">
+        <f t="shared" si="10"/>
+        <v>29.826049243395659</v>
+      </c>
       <c r="S17" s="1">
         <v>12</v>
       </c>
       <c r="T17" s="1"/>
-      <c r="U17" s="108">
+      <c r="U17" s="74">
         <v>37</v>
       </c>
-      <c r="V17" s="112">
+      <c r="V17" s="78">
         <v>37</v>
       </c>
       <c r="W17" s="1"/>
@@ -4533,24 +4581,24 @@
         <v>13</v>
       </c>
       <c r="B18" s="49">
-        <f t="shared" ref="B18:B25" si="10">B17+0.15</f>
+        <f t="shared" ref="B18:B25" si="12">B17+0.15</f>
         <v>1.9500000000000002</v>
       </c>
       <c r="C18" s="68"/>
       <c r="D18" s="48">
-        <f>$J$11+A18*EXP(A18/10)</f>
-        <v>117.70085667905018</v>
+        <f t="shared" si="2"/>
+        <v>158</v>
       </c>
       <c r="E18" s="48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>95.790339917193066</v>
       </c>
       <c r="F18" s="48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5747.4203950315841</v>
       </c>
       <c r="G18" s="48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>78.270861636279875</v>
       </c>
       <c r="I18" s="1"/>
@@ -4559,12 +4607,12 @@
         <v>13</v>
       </c>
       <c r="M18" s="1"/>
-      <c r="N18" s="108">
-        <f t="shared" si="7"/>
+      <c r="N18" s="74">
+        <f t="shared" si="8"/>
         <v>6630</v>
       </c>
-      <c r="O18" s="114">
-        <f t="shared" si="8"/>
+      <c r="O18" s="80">
+        <f t="shared" si="9"/>
         <v>5447</v>
       </c>
       <c r="P18" s="1"/>
@@ -4572,14 +4620,18 @@
         <f t="shared" si="1"/>
         <v>3898.5</v>
       </c>
+      <c r="R18" s="64">
+        <f t="shared" si="10"/>
+        <v>31.308344654511949</v>
+      </c>
       <c r="S18" s="1">
         <v>13</v>
       </c>
       <c r="T18" s="1"/>
-      <c r="U18" s="108">
+      <c r="U18" s="74">
         <v>40</v>
       </c>
-      <c r="V18" s="112">
+      <c r="V18" s="78">
         <v>40</v>
       </c>
       <c r="W18" s="1"/>
@@ -4592,24 +4644,24 @@
         <v>14</v>
       </c>
       <c r="B19" s="49">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>2.1</v>
       </c>
       <c r="C19" s="68"/>
       <c r="D19" s="48">
-        <f>$J$11+A19*EXP(A19/10)</f>
-        <v>126.77279953582544</v>
+        <f t="shared" si="2"/>
+        <v>164</v>
       </c>
       <c r="E19" s="48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>108.11545195869232</v>
       </c>
       <c r="F19" s="48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6486.927117521539</v>
       </c>
       <c r="G19" s="48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>75.687741498674228</v>
       </c>
       <c r="I19" s="1"/>
@@ -4618,12 +4670,12 @@
         <v>14</v>
       </c>
       <c r="M19" s="1"/>
-      <c r="N19" s="108">
-        <f t="shared" si="7"/>
+      <c r="N19" s="74">
+        <f t="shared" si="8"/>
         <v>7560</v>
       </c>
-      <c r="O19" s="114">
-        <f t="shared" si="8"/>
+      <c r="O19" s="80">
+        <f t="shared" si="9"/>
         <v>6244</v>
       </c>
       <c r="P19" s="1"/>
@@ -4631,14 +4683,18 @@
         <f t="shared" si="1"/>
         <v>4372</v>
       </c>
+      <c r="R19" s="64">
+        <f t="shared" si="10"/>
+        <v>32.545728844429917</v>
+      </c>
       <c r="S19" s="1">
         <v>14</v>
       </c>
       <c r="T19" s="1"/>
-      <c r="U19" s="108">
+      <c r="U19" s="74">
         <v>43</v>
       </c>
-      <c r="V19" s="112">
+      <c r="V19" s="78">
         <v>43</v>
       </c>
       <c r="W19" s="1"/>
@@ -4651,24 +4707,24 @@
         <v>15</v>
       </c>
       <c r="B20" s="49">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>2.25</v>
       </c>
       <c r="C20" s="68"/>
       <c r="D20" s="48">
-        <f>$J$11+A20*EXP(A20/10)</f>
-        <v>137.22533605507095</v>
+        <f t="shared" si="2"/>
+        <v>170</v>
       </c>
       <c r="E20" s="48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>122.52108200006279</v>
       </c>
       <c r="F20" s="48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7351.2649200037677</v>
       </c>
       <c r="G20" s="48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>72.817506039296532</v>
       </c>
       <c r="I20" s="1"/>
@@ -4677,12 +4733,12 @@
         <v>15</v>
       </c>
       <c r="M20" s="1"/>
-      <c r="N20" s="108">
-        <f t="shared" si="7"/>
+      <c r="N20" s="74">
+        <f t="shared" si="8"/>
         <v>8580</v>
       </c>
-      <c r="O20" s="114">
-        <f t="shared" si="8"/>
+      <c r="O20" s="80">
+        <f t="shared" si="9"/>
         <v>7125</v>
       </c>
       <c r="P20" s="1"/>
@@ -4690,14 +4746,18 @@
         <f t="shared" si="1"/>
         <v>4887.5</v>
       </c>
+      <c r="R20" s="64">
+        <f t="shared" si="10"/>
+        <v>33.496052778076404</v>
+      </c>
       <c r="S20" s="1">
         <v>15</v>
       </c>
       <c r="T20" s="1"/>
-      <c r="U20" s="108">
+      <c r="U20" s="74">
         <v>46</v>
       </c>
-      <c r="V20" s="112">
+      <c r="V20" s="78">
         <v>46</v>
       </c>
       <c r="W20" s="1"/>
@@ -4710,36 +4770,36 @@
         <v>16</v>
       </c>
       <c r="B21" s="49">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>2.4</v>
       </c>
       <c r="C21" s="68"/>
       <c r="D21" s="48">
-        <f>$J$11+A21*EXP(A21/10)</f>
-        <v>149.24851879032184</v>
+        <f t="shared" si="2"/>
+        <v>176</v>
       </c>
       <c r="E21" s="48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>139.59815003314424</v>
       </c>
       <c r="F21" s="48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8375.8890019886549</v>
       </c>
       <c r="G21" s="48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>69.608083904850105</v>
       </c>
       <c r="L21" s="1">
         <v>16</v>
       </c>
       <c r="M21" s="1"/>
-      <c r="N21" s="108">
-        <f t="shared" si="7"/>
+      <c r="N21" s="74">
+        <f t="shared" si="8"/>
         <v>9696</v>
       </c>
-      <c r="O21" s="114">
-        <f t="shared" si="8"/>
+      <c r="O21" s="80">
+        <f t="shared" si="9"/>
         <v>8096</v>
       </c>
       <c r="P21" s="1"/>
@@ -4747,14 +4807,18 @@
         <f t="shared" si="1"/>
         <v>5448</v>
       </c>
+      <c r="R21" s="64">
+        <f t="shared" si="10"/>
+        <v>34.107961113376547</v>
+      </c>
       <c r="S21" s="1">
         <v>16</v>
       </c>
       <c r="T21" s="1"/>
-      <c r="U21" s="108">
+      <c r="U21" s="74">
         <v>49</v>
       </c>
-      <c r="V21" s="112">
+      <c r="V21" s="78">
         <v>49</v>
       </c>
       <c r="W21" s="1"/>
@@ -4767,36 +4831,36 @@
         <v>17</v>
       </c>
       <c r="B22" s="49">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>2.5499999999999998</v>
       </c>
       <c r="C22" s="68"/>
       <c r="D22" s="48">
-        <f>$J$11+A22*EXP(A22/10)</f>
-        <v>163.05710565936238</v>
+        <f t="shared" si="2"/>
+        <v>182</v>
       </c>
       <c r="E22" s="48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>160.10541234668784</v>
       </c>
       <c r="F22" s="48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9606.3247408012703</v>
       </c>
       <c r="G22" s="48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>65.997960059905978</v>
       </c>
       <c r="L22" s="1">
         <v>17</v>
       </c>
       <c r="M22" s="1"/>
-      <c r="N22" s="108">
-        <f t="shared" si="7"/>
+      <c r="N22" s="74">
+        <f t="shared" si="8"/>
         <v>10914</v>
       </c>
-      <c r="O22" s="114">
-        <f t="shared" si="8"/>
+      <c r="O22" s="80">
+        <f t="shared" si="9"/>
         <v>9163</v>
       </c>
       <c r="P22" s="1"/>
@@ -4804,14 +4868,18 @@
         <f t="shared" si="1"/>
         <v>6056.5</v>
       </c>
+      <c r="R22" s="64">
+        <f t="shared" si="10"/>
+        <v>34.318939231151106</v>
+      </c>
       <c r="S22" s="1">
         <v>17</v>
       </c>
       <c r="T22" s="1"/>
-      <c r="U22" s="108">
+      <c r="U22" s="74">
         <v>52</v>
       </c>
-      <c r="V22" s="112">
+      <c r="V22" s="78">
         <v>52</v>
       </c>
       <c r="W22" s="1"/>
@@ -4824,36 +4892,36 @@
         <v>18</v>
       </c>
       <c r="B23" s="49">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>2.6999999999999997</v>
       </c>
       <c r="C23" s="68"/>
       <c r="D23" s="48">
-        <f>$J$11+A23*EXP(A23/10)</f>
-        <v>178.89365435943304</v>
+        <f t="shared" si="2"/>
+        <v>188</v>
       </c>
       <c r="E23" s="48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>185.01713130052181</v>
       </c>
       <c r="F23" s="48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>11101.027878031309</v>
       </c>
       <c r="G23" s="48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>61.914463076812325</v>
       </c>
       <c r="L23" s="1">
         <v>18</v>
       </c>
       <c r="M23" s="1"/>
-      <c r="N23" s="108">
-        <f t="shared" si="7"/>
+      <c r="N23" s="74">
+        <f t="shared" si="8"/>
         <v>12240</v>
       </c>
-      <c r="O23" s="114">
-        <f t="shared" si="8"/>
+      <c r="O23" s="80">
+        <f t="shared" si="9"/>
         <v>10332</v>
       </c>
       <c r="P23" s="1"/>
@@ -4861,14 +4929,18 @@
         <f t="shared" si="1"/>
         <v>6716</v>
       </c>
+      <c r="R23" s="64">
+        <f t="shared" si="10"/>
+        <v>34.052954692246779</v>
+      </c>
       <c r="S23" s="1">
         <v>18</v>
       </c>
       <c r="T23" s="1"/>
-      <c r="U23" s="108">
+      <c r="U23" s="74">
         <v>55</v>
       </c>
-      <c r="V23" s="112">
+      <c r="V23" s="78">
         <v>55</v>
       </c>
       <c r="W23" s="1"/>
@@ -4881,36 +4953,36 @@
         <v>19</v>
       </c>
       <c r="B24" s="49">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>2.8499999999999996</v>
       </c>
       <c r="C24" s="68"/>
       <c r="D24" s="48">
-        <f>$J$11+A24*EXP(A24/10)</f>
-        <v>197.0319944033061</v>
+        <f t="shared" si="2"/>
+        <v>194</v>
       </c>
       <c r="E24" s="48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>215.58428452718766</v>
       </c>
       <c r="F24" s="48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12935.05707163126</v>
       </c>
       <c r="G24" s="48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>57.271741807794839</v>
       </c>
       <c r="L24" s="1">
         <v>19</v>
       </c>
       <c r="M24" s="1"/>
-      <c r="N24" s="108">
-        <f t="shared" si="7"/>
+      <c r="N24" s="74">
+        <f t="shared" si="8"/>
         <v>13680</v>
       </c>
-      <c r="O24" s="114">
-        <f t="shared" si="8"/>
+      <c r="O24" s="80">
+        <f t="shared" si="9"/>
         <v>11609</v>
       </c>
       <c r="P24" s="1"/>
@@ -4918,14 +4990,18 @@
         <f t="shared" si="1"/>
         <v>7429.5</v>
       </c>
+      <c r="R24" s="64">
+        <f t="shared" si="10"/>
+        <v>33.217610248521005</v>
+      </c>
       <c r="S24" s="1">
         <v>19</v>
       </c>
       <c r="T24" s="1"/>
-      <c r="U24" s="108">
+      <c r="U24" s="74">
         <v>58</v>
       </c>
-      <c r="V24" s="112">
+      <c r="V24" s="78">
         <v>58</v>
       </c>
       <c r="W24" s="1"/>
@@ -4938,36 +5014,36 @@
         <v>20</v>
       </c>
       <c r="B25" s="49">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>2.9999999999999996</v>
       </c>
       <c r="C25" s="68"/>
       <c r="D25" s="48">
-        <f>$J$11+A25*EXP(A25/10)</f>
-        <v>217.78112197861302</v>
+        <f t="shared" si="2"/>
+        <v>200</v>
       </c>
       <c r="E25" s="48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>253.4131591025766</v>
       </c>
       <c r="F25" s="48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>15204.789546154596</v>
       </c>
       <c r="G25" s="48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>51.968375105473854</v>
       </c>
       <c r="L25" s="1">
         <v>20</v>
       </c>
       <c r="M25" s="1"/>
-      <c r="N25" s="108">
-        <f t="shared" si="7"/>
+      <c r="N25" s="74">
+        <f t="shared" si="8"/>
         <v>15240</v>
       </c>
-      <c r="O25" s="114">
-        <f t="shared" si="8"/>
+      <c r="O25" s="80">
+        <f t="shared" si="9"/>
         <v>13000</v>
       </c>
       <c r="P25" s="1"/>
@@ -4975,14 +5051,18 @@
         <f t="shared" si="1"/>
         <v>8200</v>
       </c>
+      <c r="R25" s="64">
+        <f t="shared" si="10"/>
+        <v>31.700708814339052</v>
+      </c>
       <c r="S25" s="1">
         <v>20</v>
       </c>
       <c r="T25" s="1"/>
-      <c r="U25" s="108">
+      <c r="U25" s="74">
         <v>61</v>
       </c>
-      <c r="V25" s="112">
+      <c r="V25" s="78">
         <v>61</v>
       </c>
       <c r="W25" s="1"/>
@@ -4994,11 +5074,11 @@
       <c r="L26" s="1">
         <v>21</v>
       </c>
-      <c r="O26" s="107"/>
+      <c r="O26" s="73"/>
       <c r="S26" s="1">
         <v>21</v>
       </c>
-      <c r="V26" s="107"/>
+      <c r="V26" s="73"/>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="L27" s="1">
@@ -5007,6 +5087,9 @@
       <c r="S27" s="1">
         <v>22</v>
       </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="R28" s="64"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Wall + Miller + Onager
</commit_message>
<xml_diff>
--- a/Equilibrage.xlsx
+++ b/Equilibrage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilisateur\Documents\Github\Dukes Of The Realm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB40CB2-8BCB-4C93-AB2D-FCD93B869BDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4B2F46C-28ED-4A99-BEA6-62FBBD4033E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Equi V.1" sheetId="1" r:id="rId1"/>
@@ -823,7 +823,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -953,9 +953,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1027,12 +1024,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1075,13 +1066,58 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1091,60 +1127,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1161,6 +1143,30 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1605,14 +1611,14 @@
       <c r="F9" s="2"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="83" t="s">
+      <c r="I9" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="J9" s="83"/>
-      <c r="K9" s="83"/>
-      <c r="L9" s="83"/>
-      <c r="M9" s="83"/>
-      <c r="N9" s="83"/>
+      <c r="J9" s="80"/>
+      <c r="K9" s="80"/>
+      <c r="L9" s="80"/>
+      <c r="M9" s="80"/>
+      <c r="N9" s="80"/>
     </row>
     <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
@@ -1632,12 +1638,12 @@
       <c r="G10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="83"/>
-      <c r="J10" s="83"/>
-      <c r="K10" s="83"/>
-      <c r="L10" s="83"/>
-      <c r="M10" s="83"/>
-      <c r="N10" s="83"/>
+      <c r="I10" s="80"/>
+      <c r="J10" s="80"/>
+      <c r="K10" s="80"/>
+      <c r="L10" s="80"/>
+      <c r="M10" s="80"/>
+      <c r="N10" s="80"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
@@ -1667,12 +1673,12 @@
         <f>G3</f>
         <v>65</v>
       </c>
-      <c r="I11" s="83"/>
-      <c r="J11" s="83"/>
-      <c r="K11" s="83"/>
-      <c r="L11" s="83"/>
-      <c r="M11" s="83"/>
-      <c r="N11" s="83"/>
+      <c r="I11" s="80"/>
+      <c r="J11" s="80"/>
+      <c r="K11" s="80"/>
+      <c r="L11" s="80"/>
+      <c r="M11" s="80"/>
+      <c r="N11" s="80"/>
     </row>
     <row r="12" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
@@ -1703,14 +1709,14 @@
         <v>100</v>
       </c>
       <c r="H12" s="1"/>
-      <c r="I12" s="82" t="s">
+      <c r="I12" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="J12" s="82"/>
-      <c r="K12" s="82"/>
-      <c r="L12" s="82"/>
-      <c r="M12" s="82"/>
-      <c r="N12" s="82"/>
+      <c r="J12" s="79"/>
+      <c r="K12" s="79"/>
+      <c r="L12" s="79"/>
+      <c r="M12" s="79"/>
+      <c r="N12" s="79"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
@@ -1741,12 +1747,12 @@
         <v>35</v>
       </c>
       <c r="H13" s="1"/>
-      <c r="I13" s="82"/>
-      <c r="J13" s="82"/>
-      <c r="K13" s="82"/>
-      <c r="L13" s="82"/>
-      <c r="M13" s="82"/>
-      <c r="N13" s="82"/>
+      <c r="I13" s="79"/>
+      <c r="J13" s="79"/>
+      <c r="K13" s="79"/>
+      <c r="L13" s="79"/>
+      <c r="M13" s="79"/>
+      <c r="N13" s="79"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
@@ -1757,12 +1763,12 @@
       <c r="F14" s="2"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="82"/>
-      <c r="J14" s="82"/>
-      <c r="K14" s="82"/>
-      <c r="L14" s="82"/>
-      <c r="M14" s="82"/>
-      <c r="N14" s="82"/>
+      <c r="I14" s="79"/>
+      <c r="J14" s="79"/>
+      <c r="K14" s="79"/>
+      <c r="L14" s="79"/>
+      <c r="M14" s="79"/>
+      <c r="N14" s="79"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
@@ -1771,12 +1777,12 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="82"/>
-      <c r="J15" s="82"/>
-      <c r="K15" s="82"/>
-      <c r="L15" s="82"/>
-      <c r="M15" s="82"/>
-      <c r="N15" s="82"/>
+      <c r="I15" s="79"/>
+      <c r="J15" s="79"/>
+      <c r="K15" s="79"/>
+      <c r="L15" s="79"/>
+      <c r="M15" s="79"/>
+      <c r="N15" s="79"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
@@ -1956,8 +1962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D1AB80D-11E3-4393-9ABD-01470CEC1085}">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1986,14 +1992,14 @@
       <c r="D2" s="44"/>
       <c r="E2" s="44"/>
       <c r="F2" s="44"/>
-      <c r="G2" s="44">
+      <c r="G2" s="117">
         <v>0.8</v>
       </c>
-      <c r="H2" s="45">
+      <c r="H2" s="116">
         <v>1.2</v>
       </c>
-      <c r="I2" s="45">
-        <v>2.5</v>
+      <c r="I2" s="116">
+        <v>1.5</v>
       </c>
       <c r="J2" s="44"/>
       <c r="K2" s="44"/>
@@ -2002,252 +2008,253 @@
       <c r="A3" s="44"/>
       <c r="B3" s="44"/>
       <c r="C3" s="44"/>
-      <c r="D3" s="47" t="s">
+      <c r="D3" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="47" t="s">
+      <c r="E3" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="47" t="s">
+      <c r="F3" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="47" t="s">
+      <c r="G3" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="47" t="s">
+      <c r="H3" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="50" t="s">
+      <c r="I3" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="50" t="s">
+      <c r="J3" s="49" t="s">
         <v>15</v>
       </c>
       <c r="K3" s="44"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="44"/>
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="52" t="s">
+      <c r="C4" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="47">
+      <c r="D4" s="46">
         <v>64</v>
       </c>
-      <c r="E4" s="47">
+      <c r="E4" s="46">
         <v>1</v>
       </c>
-      <c r="F4" s="54">
+      <c r="F4" s="53">
         <v>25</v>
       </c>
-      <c r="G4" s="46">
+      <c r="G4" s="45">
         <f>(40*G2)*G1</f>
         <v>32</v>
       </c>
-      <c r="H4" s="46">
+      <c r="H4" s="45">
         <f>20*H2</f>
         <v>24</v>
       </c>
-      <c r="I4" s="72">
+      <c r="I4" s="113">
         <f>0.45*I2</f>
-        <v>1.125</v>
-      </c>
-      <c r="J4" s="47">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="J4" s="46">
         <v>65</v>
       </c>
-      <c r="K4" s="66"/>
+      <c r="K4" s="65"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="44"/>
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="52" t="s">
+      <c r="C5" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="47">
+      <c r="D5" s="46">
         <v>128</v>
       </c>
-      <c r="E5" s="47">
+      <c r="E5" s="46">
         <v>1</v>
       </c>
-      <c r="F5" s="54">
+      <c r="F5" s="53">
         <v>25</v>
       </c>
-      <c r="G5" s="46">
+      <c r="G5" s="45">
         <f>(75*G2)*G1</f>
         <v>60</v>
       </c>
-      <c r="H5" s="46">
+      <c r="H5" s="45">
         <f>35*H2</f>
         <v>42</v>
       </c>
-      <c r="I5" s="72">
+      <c r="I5" s="113">
         <f>1.5*I2</f>
-        <v>3.75</v>
-      </c>
-      <c r="J5" s="47">
+        <v>2.25</v>
+      </c>
+      <c r="J5" s="46">
         <v>55</v>
       </c>
-      <c r="K5" s="66"/>
+      <c r="K5" s="65"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="44"/>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="51" t="s">
+      <c r="C6" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="47">
+      <c r="D6" s="46">
         <v>164</v>
       </c>
-      <c r="E6" s="47">
+      <c r="E6" s="46">
         <v>2</v>
       </c>
-      <c r="F6" s="54">
+      <c r="F6" s="53">
         <v>20</v>
       </c>
-      <c r="G6" s="46">
+      <c r="G6" s="45">
         <f>(77*G2)*G1</f>
         <v>61.6</v>
       </c>
-      <c r="H6" s="46">
+      <c r="H6" s="45">
         <f>85*H2</f>
         <v>102</v>
       </c>
-      <c r="I6" s="72">
+      <c r="I6" s="113">
         <f>2.05*I2</f>
-        <v>5.125</v>
-      </c>
-      <c r="J6" s="47">
+        <v>3.0749999999999997</v>
+      </c>
+      <c r="J6" s="46">
         <v>100</v>
       </c>
-      <c r="K6" s="66"/>
+      <c r="K6" s="65"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="44"/>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="51" t="s">
+      <c r="C7" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="47">
+      <c r="D7" s="46">
         <v>80</v>
       </c>
-      <c r="E7" s="47">
+      <c r="E7" s="46">
         <v>1</v>
       </c>
-      <c r="F7" s="54">
+      <c r="F7" s="53">
         <v>15</v>
       </c>
-      <c r="G7" s="46">
+      <c r="G7" s="45">
         <f>(20*G2)*G1</f>
         <v>16</v>
       </c>
-      <c r="H7" s="46">
+      <c r="H7" s="45">
         <f>60*H2</f>
         <v>72</v>
       </c>
-      <c r="I7" s="72">
+      <c r="I7" s="113">
         <f>0.75*I2</f>
-        <v>1.875</v>
-      </c>
-      <c r="J7" s="47">
+        <v>1.125</v>
+      </c>
+      <c r="J7" s="46">
         <v>65</v>
       </c>
-      <c r="K7" s="66"/>
+      <c r="K7" s="65"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="44"/>
-      <c r="B8" s="53" t="s">
+      <c r="B8" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="53" t="s">
+      <c r="C8" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="47">
+      <c r="D8" s="46">
         <v>192</v>
       </c>
-      <c r="E8" s="47">
+      <c r="E8" s="46">
         <v>3</v>
       </c>
-      <c r="F8" s="54">
+      <c r="F8" s="53">
         <v>10</v>
       </c>
-      <c r="G8" s="46">
+      <c r="G8" s="45">
         <f>(24*G2)*G1</f>
         <v>19.200000000000003</v>
       </c>
-      <c r="H8" s="46">
-        <f>30*H2</f>
-        <v>36</v>
-      </c>
-      <c r="I8" s="72">
+      <c r="H8" s="45">
+        <f>8*H2</f>
+        <v>9.6</v>
+      </c>
+      <c r="I8" s="113">
         <f>3*I2</f>
-        <v>7.5</v>
-      </c>
-      <c r="J8" s="47">
+        <v>4.5</v>
+      </c>
+      <c r="J8" s="46">
         <v>35</v>
       </c>
-      <c r="K8" s="66"/>
+      <c r="K8" s="65"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="44"/>
-      <c r="B9" s="53" t="s">
+      <c r="B9" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="53" t="s">
+      <c r="C9" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="47">
+      <c r="D9" s="46">
         <v>80</v>
       </c>
-      <c r="E9" s="47">
+      <c r="E9" s="46">
         <v>2</v>
       </c>
-      <c r="F9" s="54">
+      <c r="F9" s="53">
         <v>5</v>
       </c>
-      <c r="G9" s="46">
+      <c r="G9" s="45">
         <f>(8*G2)*G1</f>
         <v>6.4</v>
       </c>
-      <c r="H9" s="46">
+      <c r="H9" s="45">
         <f>5*H2</f>
         <v>6</v>
       </c>
-      <c r="I9" s="72">
+      <c r="I9" s="113">
         <f>0.875*I2</f>
-        <v>2.1875</v>
-      </c>
-      <c r="J9" s="47">
+        <v>1.3125</v>
+      </c>
+      <c r="J9" s="46">
         <v>80</v>
       </c>
-      <c r="K9" s="66"/>
+      <c r="K9" s="65"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="44"/>
+      <c r="I10" s="62"/>
       <c r="K10" s="44"/>
     </row>
     <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="44"/>
       <c r="B11" s="44"/>
-      <c r="C11" s="56" t="s">
+      <c r="C11" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="57">
+      <c r="D11" s="56">
         <v>640</v>
       </c>
-      <c r="E11" s="58" t="s">
+      <c r="E11" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="55"/>
+      <c r="F11" s="54"/>
       <c r="H11" s="44"/>
-      <c r="I11" s="44"/>
+      <c r="I11" s="114"/>
       <c r="J11" s="44"/>
       <c r="K11" s="44"/>
     </row>
@@ -2257,10 +2264,10 @@
       <c r="C12" s="44"/>
       <c r="D12" s="44"/>
       <c r="E12" s="44"/>
-      <c r="F12" s="55"/>
+      <c r="F12" s="54"/>
       <c r="G12" s="44"/>
       <c r="H12" s="44"/>
-      <c r="I12" s="44"/>
+      <c r="I12" s="114"/>
       <c r="J12" s="44"/>
       <c r="K12" s="44"/>
     </row>
@@ -2268,101 +2275,101 @@
       <c r="A13" s="44"/>
       <c r="B13" s="44"/>
       <c r="C13" s="44"/>
-      <c r="D13" s="47" t="s">
+      <c r="D13" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="E13" s="47" t="s">
+      <c r="E13" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="F13" s="54" t="s">
+      <c r="F13" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="G13" s="47" t="s">
+      <c r="G13" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="H13" s="47" t="s">
+      <c r="H13" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="I13" s="47" t="s">
+      <c r="I13" s="113" t="s">
         <v>10</v>
       </c>
-      <c r="J13" s="47" t="s">
+      <c r="J13" s="46" t="s">
         <v>8</v>
       </c>
       <c r="K13" s="44"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="44"/>
-      <c r="B14" s="46">
+      <c r="B14" s="45">
         <f>D11/D4</f>
         <v>10</v>
       </c>
-      <c r="C14" s="52" t="s">
+      <c r="C14" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="47">
+      <c r="D14" s="46">
         <f>D4*B14</f>
         <v>640</v>
       </c>
-      <c r="E14" s="46">
+      <c r="E14" s="45">
         <f>E4*B14</f>
         <v>10</v>
       </c>
-      <c r="F14" s="54">
+      <c r="F14" s="53">
         <f t="shared" ref="F14:F19" si="0">F4</f>
         <v>25</v>
       </c>
-      <c r="G14" s="46">
+      <c r="G14" s="45">
         <f>$B14*G4</f>
         <v>320</v>
       </c>
-      <c r="H14" s="46">
+      <c r="H14" s="45">
         <f t="shared" ref="H14:H19" si="1">H4*B14</f>
         <v>240</v>
       </c>
-      <c r="I14" s="72">
+      <c r="I14" s="113">
         <f t="shared" ref="I14:I19" si="2">I4*B14</f>
-        <v>11.25</v>
-      </c>
-      <c r="J14" s="46">
+        <v>6.75</v>
+      </c>
+      <c r="J14" s="45">
         <v>65</v>
       </c>
       <c r="K14" s="44"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="44"/>
-      <c r="B15" s="48">
+      <c r="B15" s="47">
         <f>D11/D5</f>
         <v>5</v>
       </c>
-      <c r="C15" s="52" t="s">
+      <c r="C15" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="49">
+      <c r="D15" s="48">
         <f>B15*D5</f>
         <v>640</v>
       </c>
-      <c r="E15" s="46">
+      <c r="E15" s="45">
         <f t="shared" ref="E15:E19" si="3">E5*B15</f>
         <v>5</v>
       </c>
-      <c r="F15" s="54">
+      <c r="F15" s="53">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="G15" s="46">
+      <c r="G15" s="45">
         <f>$B15*G5</f>
         <v>300</v>
       </c>
-      <c r="H15" s="46">
+      <c r="H15" s="45">
         <f t="shared" si="1"/>
         <v>210</v>
       </c>
-      <c r="I15" s="72">
+      <c r="I15" s="113">
         <f t="shared" si="2"/>
-        <v>18.75</v>
-      </c>
-      <c r="J15" s="48">
+        <v>11.25</v>
+      </c>
+      <c r="J15" s="47">
         <f>J5</f>
         <v>55</v>
       </c>
@@ -2370,426 +2377,426 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="44"/>
-      <c r="B16" s="46">
+      <c r="B16" s="45">
         <f>D11/D6</f>
         <v>3.9024390243902438</v>
       </c>
-      <c r="C16" s="51" t="s">
+      <c r="C16" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="47">
+      <c r="D16" s="46">
         <f>D6*B16</f>
         <v>640</v>
       </c>
-      <c r="E16" s="46">
+      <c r="E16" s="45">
         <f t="shared" si="3"/>
         <v>7.8048780487804876</v>
       </c>
-      <c r="F16" s="54">
+      <c r="F16" s="53">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="G16" s="46">
+      <c r="G16" s="45">
         <f>$B16*G6</f>
         <v>240.39024390243901</v>
       </c>
-      <c r="H16" s="46">
+      <c r="H16" s="45">
         <f t="shared" si="1"/>
         <v>398.04878048780489</v>
       </c>
-      <c r="I16" s="72">
+      <c r="I16" s="113">
         <f t="shared" si="2"/>
-        <v>20</v>
-      </c>
-      <c r="J16" s="46">
+        <v>11.999999999999998</v>
+      </c>
+      <c r="J16" s="45">
         <v>100</v>
       </c>
       <c r="K16" s="44"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="48">
+      <c r="B17" s="47">
         <f>D11/D7</f>
         <v>8</v>
       </c>
-      <c r="C17" s="51" t="s">
+      <c r="C17" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="49">
+      <c r="D17" s="48">
         <f>B17*D7</f>
         <v>640</v>
       </c>
-      <c r="E17" s="46">
+      <c r="E17" s="45">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="F17" s="54">
+      <c r="F17" s="53">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="G17" s="46">
+      <c r="G17" s="45">
         <f>$B17*G7</f>
         <v>128</v>
       </c>
-      <c r="H17" s="46">
+      <c r="H17" s="45">
         <f t="shared" si="1"/>
         <v>576</v>
       </c>
-      <c r="I17" s="72">
+      <c r="I17" s="113">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="J17" s="47">
+        <f>J7</f>
+        <v>65</v>
+      </c>
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B18" s="45">
+        <f>D11/D8</f>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="C18" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="46">
+        <f>D8*B18</f>
+        <v>640</v>
+      </c>
+      <c r="E18" s="45">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="F18" s="53">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G18" s="45">
+        <f>$B18*G8</f>
+        <v>64.000000000000014</v>
+      </c>
+      <c r="H18" s="45">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="I18" s="113">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="J17" s="48">
-        <f>J7</f>
-        <v>65</v>
-      </c>
-      <c r="K17" s="1"/>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="46">
-        <f>D11/D8</f>
-        <v>3.3333333333333335</v>
-      </c>
-      <c r="C18" s="53" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="47">
-        <f>D8*B18</f>
-        <v>640</v>
-      </c>
-      <c r="E18" s="46">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="F18" s="54">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="G18" s="46">
-        <f>$B18*G8</f>
-        <v>64.000000000000014</v>
-      </c>
-      <c r="H18" s="46">
-        <f t="shared" si="1"/>
-        <v>120</v>
-      </c>
-      <c r="I18" s="72">
-        <f t="shared" si="2"/>
-        <v>25</v>
-      </c>
-      <c r="J18" s="46">
+      <c r="J18" s="45">
         <v>35</v>
       </c>
       <c r="K18" s="44"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="48">
+      <c r="B19" s="47">
         <f>D11/D9</f>
         <v>8</v>
       </c>
-      <c r="C19" s="62" t="s">
+      <c r="C19" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="49">
+      <c r="D19" s="48">
         <f>B19*D9</f>
         <v>640</v>
       </c>
-      <c r="E19" s="46">
+      <c r="E19" s="45">
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
-      <c r="F19" s="54">
+      <c r="F19" s="53">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G19" s="46">
+      <c r="G19" s="45">
         <f>G9*B19</f>
         <v>51.2</v>
       </c>
-      <c r="H19" s="48">
+      <c r="H19" s="47">
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="I19" s="71">
+      <c r="I19" s="115">
         <f t="shared" si="2"/>
-        <v>17.5</v>
-      </c>
-      <c r="J19" s="48">
+        <v>10.5</v>
+      </c>
+      <c r="J19" s="47">
         <f>J9</f>
         <v>80</v>
       </c>
     </row>
     <row r="20" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I20" s="64"/>
+      <c r="I20" s="62"/>
     </row>
     <row r="21" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="59" t="s">
+      <c r="C21" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="D21" s="60">
+      <c r="D21" s="59">
         <v>250</v>
       </c>
-      <c r="E21" s="61" t="s">
+      <c r="E21" s="60" t="s">
         <v>45</v>
       </c>
-      <c r="I21" s="64"/>
+      <c r="I21" s="62"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="I22" s="64"/>
+      <c r="I22" s="62"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" s="44"/>
       <c r="C23" s="44"/>
-      <c r="D23" s="47" t="s">
+      <c r="D23" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="E23" s="47" t="s">
+      <c r="E23" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="F23" s="54" t="s">
+      <c r="F23" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="G23" s="47" t="s">
+      <c r="G23" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="H23" s="47" t="s">
+      <c r="H23" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="I23" s="72" t="s">
+      <c r="I23" s="113" t="s">
         <v>10</v>
       </c>
-      <c r="J23" s="47" t="s">
+      <c r="J23" s="46" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B24" s="46">
+      <c r="B24" s="45">
         <f>D$21/E4</f>
         <v>250</v>
       </c>
-      <c r="C24" s="52" t="s">
+      <c r="C24" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="D24" s="47">
+      <c r="D24" s="46">
         <f>$B$24*D4</f>
         <v>16000</v>
       </c>
-      <c r="E24" s="47">
+      <c r="E24" s="46">
         <f>$B24*E4</f>
         <v>250</v>
       </c>
-      <c r="F24" s="47">
+      <c r="F24" s="46">
         <f>F14</f>
         <v>25</v>
       </c>
-      <c r="G24" s="47">
+      <c r="G24" s="46">
         <f t="shared" ref="G24:H24" si="4">$B$24*G4</f>
         <v>8000</v>
       </c>
-      <c r="H24" s="47">
+      <c r="H24" s="46">
         <f t="shared" si="4"/>
         <v>6000</v>
       </c>
-      <c r="I24" s="72">
+      <c r="I24" s="113">
         <f>$B$24*I4</f>
-        <v>281.25</v>
-      </c>
-      <c r="J24" s="46">
+        <v>168.75</v>
+      </c>
+      <c r="J24" s="45">
         <f>J14</f>
         <v>65</v>
       </c>
-      <c r="K24" s="63"/>
-      <c r="L24" s="64"/>
+      <c r="K24" s="62"/>
+      <c r="L24" s="63"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="46">
+      <c r="B25" s="45">
         <f t="shared" ref="B25:B29" si="5">D$21/E5</f>
         <v>250</v>
       </c>
-      <c r="C25" s="52" t="s">
+      <c r="C25" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="D25" s="47">
+      <c r="D25" s="46">
         <f t="shared" ref="D25:D28" si="6">B25*D5</f>
         <v>32000</v>
       </c>
-      <c r="E25" s="47">
+      <c r="E25" s="46">
         <f>$B$25*E5</f>
         <v>250</v>
       </c>
-      <c r="F25" s="47">
+      <c r="F25" s="46">
         <f t="shared" ref="F25:F29" si="7">F15</f>
         <v>25</v>
       </c>
-      <c r="G25" s="47">
+      <c r="G25" s="46">
         <f t="shared" ref="G25:H25" si="8">$B$25*G5</f>
         <v>15000</v>
       </c>
-      <c r="H25" s="47">
+      <c r="H25" s="46">
         <f t="shared" si="8"/>
         <v>10500</v>
       </c>
-      <c r="I25" s="72">
+      <c r="I25" s="113">
         <f>$B$25*I5</f>
-        <v>937.5</v>
-      </c>
-      <c r="J25" s="46">
+        <v>562.5</v>
+      </c>
+      <c r="J25" s="45">
         <f t="shared" ref="J25:J29" si="9">J15</f>
         <v>55</v>
       </c>
-      <c r="K25" s="63"/>
+      <c r="K25" s="62"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="46">
+      <c r="B26" s="45">
         <f t="shared" si="5"/>
         <v>125</v>
       </c>
-      <c r="C26" s="51" t="s">
+      <c r="C26" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="D26" s="47">
+      <c r="D26" s="46">
         <f t="shared" si="6"/>
         <v>20500</v>
       </c>
-      <c r="E26" s="47">
+      <c r="E26" s="46">
         <f>$B$26*E6</f>
         <v>250</v>
       </c>
-      <c r="F26" s="47">
+      <c r="F26" s="46">
         <f t="shared" si="7"/>
         <v>20</v>
       </c>
-      <c r="G26" s="47">
+      <c r="G26" s="46">
         <f t="shared" ref="G26:I26" si="10">$B$26*G6</f>
         <v>7700</v>
       </c>
-      <c r="H26" s="47">
+      <c r="H26" s="46">
         <f t="shared" si="10"/>
         <v>12750</v>
       </c>
-      <c r="I26" s="72">
+      <c r="I26" s="113">
         <f t="shared" si="10"/>
-        <v>640.625</v>
-      </c>
-      <c r="J26" s="46">
+        <v>384.37499999999994</v>
+      </c>
+      <c r="J26" s="45">
         <f t="shared" si="9"/>
         <v>100</v>
       </c>
-      <c r="K26" s="63"/>
-      <c r="L26" s="64"/>
+      <c r="K26" s="62"/>
+      <c r="L26" s="63"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B27" s="46">
+      <c r="B27" s="45">
         <f t="shared" si="5"/>
         <v>250</v>
       </c>
-      <c r="C27" s="51" t="s">
+      <c r="C27" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="47">
+      <c r="D27" s="46">
         <f t="shared" si="6"/>
         <v>20000</v>
       </c>
-      <c r="E27" s="47">
+      <c r="E27" s="46">
         <f>$B$27*E7</f>
         <v>250</v>
       </c>
-      <c r="F27" s="47">
+      <c r="F27" s="46">
         <f t="shared" si="7"/>
         <v>15</v>
       </c>
-      <c r="G27" s="47">
+      <c r="G27" s="46">
         <f t="shared" ref="G27:H27" si="11">$B$27*G7</f>
         <v>4000</v>
       </c>
-      <c r="H27" s="47">
+      <c r="H27" s="46">
         <f t="shared" si="11"/>
         <v>18000</v>
       </c>
-      <c r="I27" s="72">
+      <c r="I27" s="113">
         <f>$B$27*I7</f>
-        <v>468.75</v>
-      </c>
-      <c r="J27" s="46">
+        <v>281.25</v>
+      </c>
+      <c r="J27" s="45">
         <f t="shared" si="9"/>
         <v>65</v>
       </c>
-      <c r="K27" s="63"/>
+      <c r="K27" s="62"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B28" s="46">
+      <c r="B28" s="45">
         <f t="shared" si="5"/>
         <v>83.333333333333329</v>
       </c>
-      <c r="C28" s="53" t="s">
+      <c r="C28" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="D28" s="47">
+      <c r="D28" s="46">
         <f t="shared" si="6"/>
         <v>16000</v>
       </c>
-      <c r="E28" s="47">
+      <c r="E28" s="46">
         <f>$B$28*E8</f>
         <v>250</v>
       </c>
-      <c r="F28" s="47">
+      <c r="F28" s="46">
         <f t="shared" si="7"/>
         <v>10</v>
       </c>
-      <c r="G28" s="47">
+      <c r="G28" s="46">
         <f t="shared" ref="G28:I28" si="12">$B$28*G8</f>
         <v>1600.0000000000002</v>
       </c>
-      <c r="H28" s="47">
+      <c r="H28" s="46">
         <f t="shared" si="12"/>
-        <v>3000</v>
-      </c>
-      <c r="I28" s="72">
+        <v>799.99999999999989</v>
+      </c>
+      <c r="I28" s="113">
         <f t="shared" si="12"/>
-        <v>625</v>
-      </c>
-      <c r="J28" s="46">
+        <v>375</v>
+      </c>
+      <c r="J28" s="45">
         <f t="shared" si="9"/>
         <v>35</v>
       </c>
-      <c r="K28" s="63"/>
+      <c r="K28" s="62"/>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B29" s="46">
+      <c r="B29" s="45">
         <f t="shared" si="5"/>
         <v>125</v>
       </c>
-      <c r="C29" s="62" t="s">
+      <c r="C29" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="D29" s="47">
+      <c r="D29" s="46">
         <f>B29*D9</f>
         <v>10000</v>
       </c>
-      <c r="E29" s="47">
+      <c r="E29" s="46">
         <f>$B$29*E9</f>
         <v>250</v>
       </c>
-      <c r="F29" s="47">
+      <c r="F29" s="46">
         <f t="shared" si="7"/>
         <v>5</v>
       </c>
-      <c r="G29" s="47">
+      <c r="G29" s="46">
         <f t="shared" ref="G29:I29" si="13">$B$29*G9</f>
         <v>800</v>
       </c>
-      <c r="H29" s="47">
+      <c r="H29" s="46">
         <f t="shared" si="13"/>
         <v>750</v>
       </c>
-      <c r="I29" s="72">
+      <c r="I29" s="113">
         <f t="shared" si="13"/>
-        <v>273.4375</v>
-      </c>
-      <c r="J29" s="46">
+        <v>164.0625</v>
+      </c>
+      <c r="J29" s="45">
         <f t="shared" si="9"/>
         <v>80</v>
       </c>
-      <c r="K29" s="63"/>
+      <c r="K29" s="62"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G14:G19">
@@ -3169,44 +3176,44 @@
   <sheetData>
     <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="110" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="89"/>
+      <c r="C3" s="111"/>
+      <c r="D3" s="111"/>
+      <c r="E3" s="111"/>
+      <c r="F3" s="112"/>
       <c r="G3" s="21"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="90" t="s">
+      <c r="B4" s="102" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="91"/>
-      <c r="D4" s="91"/>
-      <c r="E4" s="92"/>
+      <c r="C4" s="103"/>
+      <c r="D4" s="103"/>
+      <c r="E4" s="104"/>
       <c r="F4" s="29">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="102" t="s">
+      <c r="B5" s="90" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="103"/>
-      <c r="D5" s="103"/>
-      <c r="E5" s="104"/>
+      <c r="C5" s="91"/>
+      <c r="D5" s="91"/>
+      <c r="E5" s="92"/>
       <c r="F5" s="35">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="93" t="s">
+      <c r="B6" s="84" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="94"/>
-      <c r="D6" s="94"/>
-      <c r="E6" s="95"/>
+      <c r="C6" s="85"/>
+      <c r="D6" s="85"/>
+      <c r="E6" s="86"/>
       <c r="F6" s="27">
         <v>6</v>
       </c>
@@ -3223,18 +3230,18 @@
       </c>
     </row>
     <row r="8" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="93" t="s">
+      <c r="B8" s="84" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="94"/>
-      <c r="D8" s="94"/>
-      <c r="E8" s="95"/>
+      <c r="C8" s="85"/>
+      <c r="D8" s="85"/>
+      <c r="E8" s="86"/>
       <c r="F8" s="27">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="114" t="s">
+      <c r="B9" s="108" t="s">
         <v>35</v>
       </c>
       <c r="C9" s="97"/>
@@ -3245,56 +3252,56 @@
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="108" t="s">
+      <c r="B10" s="99" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="109"/>
-      <c r="D10" s="109"/>
-      <c r="E10" s="110"/>
+      <c r="C10" s="100"/>
+      <c r="D10" s="100"/>
+      <c r="E10" s="101"/>
       <c r="F10" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="115" t="s">
+      <c r="B11" s="109" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="100"/>
-      <c r="D11" s="100"/>
-      <c r="E11" s="101"/>
+      <c r="C11" s="88"/>
+      <c r="D11" s="88"/>
+      <c r="E11" s="89"/>
       <c r="F11" s="28">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="90" t="s">
+      <c r="B12" s="102" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="91"/>
-      <c r="D12" s="91"/>
-      <c r="E12" s="92"/>
+      <c r="C12" s="103"/>
+      <c r="D12" s="103"/>
+      <c r="E12" s="104"/>
       <c r="F12" s="29">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="84" t="s">
+      <c r="B13" s="81" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="85"/>
-      <c r="D13" s="85"/>
-      <c r="E13" s="86"/>
+      <c r="C13" s="82"/>
+      <c r="D13" s="82"/>
+      <c r="E13" s="83"/>
       <c r="F13" s="23">
         <v>10</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="93" t="s">
+      <c r="B14" s="84" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="94"/>
-      <c r="D14" s="94"/>
-      <c r="E14" s="95"/>
+      <c r="C14" s="85"/>
+      <c r="D14" s="85"/>
+      <c r="E14" s="86"/>
       <c r="F14" s="24">
         <v>0</v>
       </c>
@@ -3311,95 +3318,100 @@
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="108" t="s">
+      <c r="B16" s="99" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="109"/>
-      <c r="D16" s="109"/>
-      <c r="E16" s="110"/>
+      <c r="C16" s="100"/>
+      <c r="D16" s="100"/>
+      <c r="E16" s="101"/>
       <c r="F16" s="25">
         <v>20</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="99" t="s">
+      <c r="B17" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="100"/>
-      <c r="D17" s="100"/>
-      <c r="E17" s="101"/>
+      <c r="C17" s="88"/>
+      <c r="D17" s="88"/>
+      <c r="E17" s="89"/>
       <c r="F17" s="32">
         <v>0.9</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="90" t="s">
+      <c r="B18" s="102" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="91"/>
-      <c r="D18" s="91"/>
-      <c r="E18" s="92"/>
+      <c r="C18" s="103"/>
+      <c r="D18" s="103"/>
+      <c r="E18" s="104"/>
       <c r="F18" s="33">
         <v>3</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="99" t="s">
+      <c r="B19" s="87" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="100"/>
-      <c r="D19" s="100"/>
-      <c r="E19" s="101"/>
+      <c r="C19" s="88"/>
+      <c r="D19" s="88"/>
+      <c r="E19" s="89"/>
       <c r="F19" s="34">
         <v>0.66700000000000004</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="111" t="s">
+      <c r="B20" s="105" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="112"/>
-      <c r="D20" s="112"/>
-      <c r="E20" s="113"/>
+      <c r="C20" s="106"/>
+      <c r="D20" s="106"/>
+      <c r="E20" s="107"/>
       <c r="F20" s="30">
         <v>12</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="84" t="s">
+      <c r="B21" s="81" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="85"/>
-      <c r="D21" s="85"/>
-      <c r="E21" s="86"/>
+      <c r="C21" s="82"/>
+      <c r="D21" s="82"/>
+      <c r="E21" s="83"/>
       <c r="F21" s="23">
         <v>3</v>
       </c>
     </row>
     <row r="22" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="93" t="s">
+      <c r="B22" s="84" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="94"/>
-      <c r="D22" s="94"/>
-      <c r="E22" s="95"/>
+      <c r="C22" s="85"/>
+      <c r="D22" s="85"/>
+      <c r="E22" s="86"/>
       <c r="F22" s="24">
         <v>4</v>
       </c>
     </row>
     <row r="23" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="105" t="s">
+      <c r="B23" s="93" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="106"/>
-      <c r="D23" s="106"/>
-      <c r="E23" s="107"/>
+      <c r="C23" s="94"/>
+      <c r="D23" s="94"/>
+      <c r="E23" s="95"/>
       <c r="F23" s="36">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
     <mergeCell ref="B21:E21"/>
     <mergeCell ref="B22:E22"/>
     <mergeCell ref="B19:E19"/>
@@ -3416,11 +3428,6 @@
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3431,8 +3438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7358574A-592A-4C40-9736-421EE2E19A0C}">
   <dimension ref="A2:X28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView topLeftCell="H1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3450,19 +3457,19 @@
       <c r="S2" t="s">
         <v>61</v>
       </c>
-      <c r="T2" s="79">
+      <c r="T2" s="76">
         <v>0</v>
       </c>
-      <c r="U2" s="79">
+      <c r="U2" s="76">
         <v>1</v>
       </c>
-      <c r="V2" s="79">
+      <c r="V2" s="76">
         <v>1</v>
       </c>
-      <c r="W2" s="79">
+      <c r="W2" s="76">
         <v>3</v>
       </c>
-      <c r="X2" s="79">
+      <c r="X2" s="76">
         <v>6</v>
       </c>
     </row>
@@ -3491,182 +3498,182 @@
       <c r="L3" t="s">
         <v>63</v>
       </c>
-      <c r="M3" s="79">
+      <c r="M3" s="76">
         <v>200</v>
       </c>
-      <c r="N3" s="79">
+      <c r="N3" s="76">
         <v>300</v>
       </c>
-      <c r="O3" s="79">
+      <c r="O3" s="76">
         <v>250</v>
       </c>
-      <c r="P3" s="79">
+      <c r="P3" s="76">
         <v>100</v>
       </c>
-      <c r="Q3" s="79">
+      <c r="Q3" s="76">
         <v>200</v>
       </c>
       <c r="S3" t="s">
         <v>62</v>
       </c>
-      <c r="T3" s="79">
+      <c r="T3" s="76">
         <v>4</v>
       </c>
-      <c r="U3" s="79">
+      <c r="U3" s="76">
         <v>3</v>
       </c>
-      <c r="V3" s="79">
+      <c r="V3" s="76">
         <v>3</v>
       </c>
-      <c r="W3" s="79">
+      <c r="W3" s="76">
         <v>2</v>
       </c>
-      <c r="X3" s="79">
+      <c r="X3" s="76">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="49" t="s">
+      <c r="C4" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="49" t="s">
+      <c r="D4" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="E4" s="70" t="s">
+      <c r="E4" s="69" t="s">
         <v>55</v>
       </c>
-      <c r="F4" s="70" t="s">
+      <c r="F4" s="69" t="s">
         <v>55</v>
       </c>
-      <c r="G4" s="70" t="s">
+      <c r="G4" s="69" t="s">
         <v>55</v>
       </c>
-      <c r="H4" s="70" t="s">
+      <c r="H4" s="69" t="s">
         <v>58</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="L4" s="73" t="s">
+      <c r="L4" s="70" t="s">
         <v>48</v>
       </c>
-      <c r="M4" s="73" t="s">
+      <c r="M4" s="70" t="s">
         <v>49</v>
       </c>
-      <c r="N4" s="73" t="s">
+      <c r="N4" s="70" t="s">
         <v>50</v>
       </c>
-      <c r="O4" s="81" t="s">
+      <c r="O4" s="78" t="s">
         <v>55</v>
       </c>
-      <c r="P4" s="73" t="s">
+      <c r="P4" s="70" t="s">
         <v>58</v>
       </c>
-      <c r="Q4" s="73" t="s">
+      <c r="Q4" s="70" t="s">
         <v>47</v>
       </c>
-      <c r="S4" s="73" t="s">
+      <c r="S4" s="70" t="s">
         <v>48</v>
       </c>
-      <c r="T4" s="73" t="s">
+      <c r="T4" s="70" t="s">
         <v>49</v>
       </c>
-      <c r="U4" s="73" t="s">
+      <c r="U4" s="70" t="s">
         <v>50</v>
       </c>
-      <c r="V4" s="73" t="s">
+      <c r="V4" s="70" t="s">
         <v>55</v>
       </c>
-      <c r="W4" s="73" t="s">
+      <c r="W4" s="70" t="s">
         <v>58</v>
       </c>
-      <c r="X4" s="73" t="s">
+      <c r="X4" s="70" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="49">
+      <c r="A5" s="48">
         <v>0</v>
       </c>
-      <c r="B5" s="67">
+      <c r="B5" s="66">
         <v>1</v>
       </c>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="69"/>
-      <c r="H5" s="49">
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="48">
         <v>0</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="J5" s="1">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="L5" s="1">
         <v>0</v>
       </c>
-      <c r="M5" s="69"/>
-      <c r="N5" s="69"/>
-      <c r="O5" s="75"/>
-      <c r="P5" s="76">
+      <c r="M5" s="68"/>
+      <c r="N5" s="68"/>
+      <c r="O5" s="72"/>
+      <c r="P5" s="73">
         <f>100 + L6*L6*L6*L6 / 4</f>
         <v>100.25</v>
       </c>
-      <c r="Q5" s="48">
+      <c r="Q5" s="47">
         <f>200*L6 + L5*L5*(L5/2)</f>
         <v>200</v>
       </c>
       <c r="S5" s="1">
         <v>0</v>
       </c>
-      <c r="T5" s="69"/>
-      <c r="U5" s="69"/>
-      <c r="V5" s="75"/>
-      <c r="W5" s="76">
+      <c r="T5" s="68"/>
+      <c r="U5" s="68"/>
+      <c r="V5" s="72"/>
+      <c r="W5" s="73">
         <v>3</v>
       </c>
-      <c r="X5" s="48">
+      <c r="X5" s="47">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" s="49">
+      <c r="A6" s="48">
         <v>1</v>
       </c>
-      <c r="B6" s="49">
+      <c r="B6" s="48">
         <f>B5+0.05</f>
         <v>1.05</v>
       </c>
-      <c r="C6" s="65">
+      <c r="C6" s="64">
         <v>1</v>
       </c>
-      <c r="D6" s="48">
+      <c r="D6" s="47">
         <f>80+6*A6</f>
         <v>86</v>
       </c>
-      <c r="E6" s="48">
+      <c r="E6" s="47">
         <f>$E$2+A6*$E$2+EXP(A6/4)</f>
         <v>11.284025416687742</v>
       </c>
-      <c r="F6" s="48">
+      <c r="F6" s="47">
         <f>E6*60</f>
         <v>677.04152500126452</v>
       </c>
-      <c r="G6" s="48">
+      <c r="G6" s="47">
         <f>100-EXP(A6/6)-A6</f>
         <v>97.818639587134356</v>
       </c>
-      <c r="H6" s="48">
+      <c r="H6" s="47">
         <f>A6*(A6/2)+A6</f>
         <v>1.5</v>
       </c>
@@ -3679,77 +3686,77 @@
       <c r="L6" s="1">
         <v>1</v>
       </c>
-      <c r="M6" s="77">
+      <c r="M6" s="74">
         <f>200*L8+L8*L8*L8*L8/7</f>
         <v>611.57142857142856</v>
       </c>
-      <c r="N6" s="74">
+      <c r="N6" s="71">
         <f>300*L6+L6*L7*L8</f>
         <v>306</v>
       </c>
-      <c r="O6" s="80">
+      <c r="O6" s="77">
         <f>250*L6+L6*L6*L6</f>
         <v>251</v>
       </c>
-      <c r="P6" s="76">
+      <c r="P6" s="73">
         <f t="shared" ref="P6:P15" si="0">100 + L7*L7*L7*L7 / 4</f>
         <v>104</v>
       </c>
-      <c r="Q6" s="48">
+      <c r="Q6" s="47">
         <f t="shared" ref="Q6:Q25" si="1">200*L7 + L6*L6*(L6/2)</f>
         <v>400.5</v>
       </c>
-      <c r="R6" s="64">
+      <c r="R6" s="63">
         <f>V6*G6/100</f>
         <v>3.9127455834853744</v>
       </c>
       <c r="S6" s="1">
         <v>1</v>
       </c>
-      <c r="T6" s="77">
+      <c r="T6" s="74">
         <v>4</v>
       </c>
-      <c r="U6" s="74">
+      <c r="U6" s="71">
         <v>4</v>
       </c>
-      <c r="V6" s="78">
+      <c r="V6" s="75">
         <v>4</v>
       </c>
-      <c r="W6" s="76">
+      <c r="W6" s="73">
         <v>5</v>
       </c>
-      <c r="X6" s="48">
+      <c r="X6" s="47">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="49">
+      <c r="A7" s="48">
         <v>2</v>
       </c>
-      <c r="B7" s="49">
+      <c r="B7" s="48">
         <f>B6+0.05</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="C7" s="65">
+      <c r="C7" s="64">
         <v>1</v>
       </c>
-      <c r="D7" s="48">
+      <c r="D7" s="47">
         <f t="shared" ref="D7:D25" si="2">80+6*A7</f>
         <v>92</v>
       </c>
-      <c r="E7" s="48">
+      <c r="E7" s="47">
         <f t="shared" ref="E7:E25" si="3">$E$2+A7*$E$2+EXP(A7/4)</f>
         <v>16.648721270700129</v>
       </c>
-      <c r="F7" s="48">
+      <c r="F7" s="47">
         <f t="shared" ref="F7:F25" si="4">E7*60</f>
         <v>998.92327624200777</v>
       </c>
-      <c r="G7" s="48">
+      <c r="G7" s="47">
         <f t="shared" ref="G7:G25" si="5">100-EXP(A7/6)-A7</f>
         <v>96.604387574913915</v>
       </c>
-      <c r="H7" s="48">
+      <c r="H7" s="47">
         <f t="shared" ref="H7:H15" si="6">A7*(A7/2)+A7</f>
         <v>4</v>
       </c>
@@ -3762,77 +3769,77 @@
       <c r="L7" s="1">
         <v>2</v>
       </c>
-      <c r="M7" s="77">
+      <c r="M7" s="74">
         <f t="shared" ref="M7:M15" si="7">200*L9+L9*L9*L9*L9/7</f>
         <v>836.57142857142856</v>
       </c>
-      <c r="N7" s="74">
+      <c r="N7" s="71">
         <f t="shared" ref="N7:N25" si="8">300*L7+L7*L8*L9</f>
         <v>624</v>
       </c>
-      <c r="O7" s="80">
+      <c r="O7" s="77">
         <f t="shared" ref="O7:O25" si="9">250*L7+L7*L7*L7</f>
         <v>508</v>
       </c>
-      <c r="P7" s="76">
+      <c r="P7" s="73">
         <f t="shared" si="0"/>
         <v>120.25</v>
       </c>
-      <c r="Q7" s="48">
+      <c r="Q7" s="47">
         <f t="shared" si="1"/>
         <v>604</v>
       </c>
-      <c r="R7" s="64">
+      <c r="R7" s="63">
         <f t="shared" ref="R7:R25" si="10">V7*G7/100</f>
         <v>6.7623071302439737</v>
       </c>
       <c r="S7" s="1">
         <v>2</v>
       </c>
-      <c r="T7" s="77">
+      <c r="T7" s="74">
         <v>8</v>
       </c>
-      <c r="U7" s="74">
+      <c r="U7" s="71">
         <v>7</v>
       </c>
-      <c r="V7" s="78">
+      <c r="V7" s="75">
         <v>7</v>
       </c>
-      <c r="W7" s="76">
+      <c r="W7" s="73">
         <v>7</v>
       </c>
-      <c r="X7" s="48">
+      <c r="X7" s="47">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" s="49">
+      <c r="A8" s="48">
         <v>3</v>
       </c>
-      <c r="B8" s="49">
+      <c r="B8" s="48">
         <f t="shared" ref="B8:B15" si="11">B7+0.05</f>
         <v>1.1500000000000001</v>
       </c>
-      <c r="C8" s="65">
+      <c r="C8" s="64">
         <v>2</v>
       </c>
-      <c r="D8" s="48">
+      <c r="D8" s="47">
         <f t="shared" si="2"/>
         <v>98</v>
       </c>
-      <c r="E8" s="48">
+      <c r="E8" s="47">
         <f t="shared" si="3"/>
         <v>22.117000016612675</v>
       </c>
-      <c r="F8" s="48">
+      <c r="F8" s="47">
         <f t="shared" si="4"/>
         <v>1327.0200009967605</v>
       </c>
-      <c r="G8" s="48">
+      <c r="G8" s="47">
         <f t="shared" si="5"/>
         <v>95.351278729299878</v>
       </c>
-      <c r="H8" s="48">
+      <c r="H8" s="47">
         <f t="shared" si="6"/>
         <v>7.5</v>
       </c>
@@ -3845,77 +3852,77 @@
       <c r="L8" s="1">
         <v>3</v>
       </c>
-      <c r="M8" s="77">
+      <c r="M8" s="74">
         <f t="shared" si="7"/>
         <v>1089.2857142857142</v>
       </c>
-      <c r="N8" s="74">
+      <c r="N8" s="71">
         <f t="shared" si="8"/>
         <v>960</v>
       </c>
-      <c r="O8" s="80">
+      <c r="O8" s="77">
         <f t="shared" si="9"/>
         <v>777</v>
       </c>
-      <c r="P8" s="76">
+      <c r="P8" s="73">
         <f t="shared" si="0"/>
         <v>164</v>
       </c>
-      <c r="Q8" s="48">
+      <c r="Q8" s="47">
         <f t="shared" si="1"/>
         <v>813.5</v>
       </c>
-      <c r="R8" s="64">
+      <c r="R8" s="63">
         <f t="shared" si="10"/>
         <v>9.5351278729299889</v>
       </c>
       <c r="S8" s="1">
         <v>3</v>
       </c>
-      <c r="T8" s="77">
+      <c r="T8" s="74">
         <v>12</v>
       </c>
-      <c r="U8" s="74">
+      <c r="U8" s="71">
         <v>10</v>
       </c>
-      <c r="V8" s="78">
+      <c r="V8" s="75">
         <v>10</v>
       </c>
-      <c r="W8" s="76">
+      <c r="W8" s="73">
         <v>9</v>
       </c>
-      <c r="X8" s="48">
+      <c r="X8" s="47">
         <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A9" s="49">
+      <c r="A9" s="48">
         <v>4</v>
       </c>
-      <c r="B9" s="49">
+      <c r="B9" s="48">
         <f t="shared" si="11"/>
         <v>1.2000000000000002</v>
       </c>
-      <c r="C9" s="65">
+      <c r="C9" s="64">
         <v>2</v>
       </c>
-      <c r="D9" s="48">
+      <c r="D9" s="47">
         <f t="shared" si="2"/>
         <v>104</v>
       </c>
-      <c r="E9" s="48">
+      <c r="E9" s="47">
         <f t="shared" si="3"/>
         <v>27.718281828459045</v>
       </c>
-      <c r="F9" s="48">
+      <c r="F9" s="47">
         <f t="shared" si="4"/>
         <v>1663.0969097075426</v>
       </c>
-      <c r="G9" s="48">
+      <c r="G9" s="47">
         <f t="shared" si="5"/>
         <v>94.052265958945327</v>
       </c>
-      <c r="H9" s="48">
+      <c r="H9" s="47">
         <f t="shared" si="6"/>
         <v>12</v>
       </c>
@@ -3928,77 +3935,77 @@
       <c r="L9" s="1">
         <v>4</v>
       </c>
-      <c r="M9" s="77">
+      <c r="M9" s="74">
         <f t="shared" si="7"/>
         <v>1385.1428571428571</v>
       </c>
-      <c r="N9" s="74">
+      <c r="N9" s="71">
         <f t="shared" si="8"/>
         <v>1320</v>
       </c>
-      <c r="O9" s="80">
+      <c r="O9" s="77">
         <f t="shared" si="9"/>
         <v>1064</v>
       </c>
-      <c r="P9" s="76">
+      <c r="P9" s="73">
         <f t="shared" si="0"/>
         <v>256.25</v>
       </c>
-      <c r="Q9" s="48">
+      <c r="Q9" s="47">
         <f t="shared" si="1"/>
         <v>1032</v>
       </c>
-      <c r="R9" s="64">
+      <c r="R9" s="63">
         <f t="shared" si="10"/>
         <v>12.226794574662893</v>
       </c>
       <c r="S9" s="1">
         <v>4</v>
       </c>
-      <c r="T9" s="77">
+      <c r="T9" s="74">
         <v>16</v>
       </c>
-      <c r="U9" s="74">
+      <c r="U9" s="71">
         <v>13</v>
       </c>
-      <c r="V9" s="78">
+      <c r="V9" s="75">
         <v>13</v>
       </c>
-      <c r="W9" s="76">
+      <c r="W9" s="73">
         <v>11</v>
       </c>
-      <c r="X9" s="48">
+      <c r="X9" s="47">
         <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A10" s="49">
+      <c r="A10" s="48">
         <v>5</v>
       </c>
-      <c r="B10" s="49">
+      <c r="B10" s="48">
         <f t="shared" si="11"/>
         <v>1.2500000000000002</v>
       </c>
-      <c r="C10" s="65">
+      <c r="C10" s="64">
         <v>3</v>
       </c>
-      <c r="D10" s="48">
+      <c r="D10" s="47">
         <f t="shared" si="2"/>
         <v>110</v>
       </c>
-      <c r="E10" s="48">
+      <c r="E10" s="47">
         <f t="shared" si="3"/>
         <v>33.490342957461841</v>
       </c>
-      <c r="F10" s="48">
+      <c r="F10" s="47">
         <f t="shared" si="4"/>
         <v>2009.4205774477105</v>
       </c>
-      <c r="G10" s="48">
+      <c r="G10" s="47">
         <f t="shared" si="5"/>
         <v>92.699024109107171</v>
       </c>
-      <c r="H10" s="48">
+      <c r="H10" s="47">
         <f t="shared" si="6"/>
         <v>17.5</v>
       </c>
@@ -4011,236 +4018,236 @@
       <c r="L10" s="1">
         <v>5</v>
       </c>
-      <c r="M10" s="77">
+      <c r="M10" s="74">
         <f t="shared" si="7"/>
         <v>1743</v>
       </c>
-      <c r="N10" s="74">
+      <c r="N10" s="71">
         <f t="shared" si="8"/>
         <v>1710</v>
       </c>
-      <c r="O10" s="80">
+      <c r="O10" s="77">
         <f t="shared" si="9"/>
         <v>1375</v>
       </c>
-      <c r="P10" s="76">
+      <c r="P10" s="73">
         <f t="shared" si="0"/>
         <v>424</v>
       </c>
-      <c r="Q10" s="48">
+      <c r="Q10" s="47">
         <f t="shared" si="1"/>
         <v>1262.5</v>
       </c>
-      <c r="R10" s="64">
+      <c r="R10" s="63">
         <f t="shared" si="10"/>
         <v>14.831843857457148</v>
       </c>
       <c r="S10" s="1">
         <v>5</v>
       </c>
-      <c r="T10" s="77">
+      <c r="T10" s="74">
         <v>20</v>
       </c>
-      <c r="U10" s="74">
+      <c r="U10" s="71">
         <v>16</v>
       </c>
-      <c r="V10" s="78">
+      <c r="V10" s="75">
         <v>16</v>
       </c>
-      <c r="W10" s="76">
+      <c r="W10" s="73">
         <v>13</v>
       </c>
-      <c r="X10" s="48">
+      <c r="X10" s="47">
         <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A11" s="49">
+      <c r="A11" s="48">
         <v>6</v>
       </c>
-      <c r="B11" s="49">
+      <c r="B11" s="48">
         <f t="shared" si="11"/>
         <v>1.3000000000000003</v>
       </c>
-      <c r="C11" s="65">
+      <c r="C11" s="64">
         <v>3</v>
       </c>
-      <c r="D11" s="48">
+      <c r="D11" s="47">
         <f t="shared" si="2"/>
         <v>116</v>
       </c>
-      <c r="E11" s="48">
+      <c r="E11" s="47">
         <f t="shared" si="3"/>
         <v>39.481689070338064</v>
       </c>
-      <c r="F11" s="48">
+      <c r="F11" s="47">
         <f t="shared" si="4"/>
         <v>2368.901344220284</v>
       </c>
-      <c r="G11" s="48">
+      <c r="G11" s="47">
         <f t="shared" si="5"/>
         <v>91.281718171540959</v>
       </c>
-      <c r="H11" s="48">
+      <c r="H11" s="47">
         <f t="shared" si="6"/>
         <v>24</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1">
         <f>J5+J6*2+J7*3+J8+J9+J10*2</f>
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="L11" s="1">
         <v>6</v>
       </c>
-      <c r="M11" s="77">
+      <c r="M11" s="74">
         <f t="shared" si="7"/>
         <v>2185.1428571428569</v>
       </c>
-      <c r="N11" s="74">
+      <c r="N11" s="71">
         <f t="shared" si="8"/>
         <v>2136</v>
       </c>
-      <c r="O11" s="80">
+      <c r="O11" s="77">
         <f t="shared" si="9"/>
         <v>1716</v>
       </c>
-      <c r="P11" s="76">
+      <c r="P11" s="73">
         <f t="shared" si="0"/>
         <v>700.25</v>
       </c>
-      <c r="Q11" s="48">
+      <c r="Q11" s="47">
         <f t="shared" si="1"/>
         <v>1508</v>
       </c>
-      <c r="R11" s="64">
+      <c r="R11" s="63">
         <f t="shared" si="10"/>
         <v>17.343526452592783</v>
       </c>
       <c r="S11" s="1">
         <v>6</v>
       </c>
-      <c r="T11" s="77">
+      <c r="T11" s="74">
         <v>24</v>
       </c>
-      <c r="U11" s="74">
+      <c r="U11" s="71">
         <v>19</v>
       </c>
-      <c r="V11" s="78">
+      <c r="V11" s="75">
         <v>19</v>
       </c>
-      <c r="W11" s="76">
+      <c r="W11" s="73">
         <v>15</v>
       </c>
-      <c r="X11" s="48">
+      <c r="X11" s="47">
         <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A12" s="49">
+      <c r="A12" s="48">
         <v>7</v>
       </c>
-      <c r="B12" s="49">
+      <c r="B12" s="48">
         <f t="shared" si="11"/>
         <v>1.3500000000000003</v>
       </c>
-      <c r="C12" s="65">
+      <c r="C12" s="64">
         <v>4</v>
       </c>
-      <c r="D12" s="48">
+      <c r="D12" s="47">
         <f t="shared" si="2"/>
         <v>122</v>
       </c>
-      <c r="E12" s="48">
+      <c r="E12" s="47">
         <f t="shared" si="3"/>
         <v>45.754602676005732</v>
       </c>
-      <c r="F12" s="48">
+      <c r="F12" s="47">
         <f t="shared" si="4"/>
         <v>2745.2761605603437</v>
       </c>
-      <c r="G12" s="48">
+      <c r="G12" s="47">
         <f t="shared" si="5"/>
         <v>89.78872945684644</v>
       </c>
-      <c r="H12" s="48">
+      <c r="H12" s="47">
         <f t="shared" si="6"/>
         <v>31.5</v>
       </c>
       <c r="L12" s="1">
         <v>7</v>
       </c>
-      <c r="M12" s="77">
+      <c r="M12" s="74">
         <f t="shared" si="7"/>
         <v>2737.2857142857142</v>
       </c>
-      <c r="N12" s="74">
+      <c r="N12" s="71">
         <f t="shared" si="8"/>
         <v>2604</v>
       </c>
-      <c r="O12" s="80">
+      <c r="O12" s="77">
         <f t="shared" si="9"/>
         <v>2093</v>
       </c>
-      <c r="P12" s="76">
+      <c r="P12" s="73">
         <f t="shared" si="0"/>
         <v>1124</v>
       </c>
-      <c r="Q12" s="48">
+      <c r="Q12" s="47">
         <f t="shared" si="1"/>
         <v>1771.5</v>
       </c>
-      <c r="R12" s="64">
+      <c r="R12" s="63">
         <f t="shared" si="10"/>
         <v>19.753520480506218</v>
       </c>
       <c r="S12" s="1">
         <v>7</v>
       </c>
-      <c r="T12" s="77">
+      <c r="T12" s="74">
         <v>28</v>
       </c>
-      <c r="U12" s="74">
+      <c r="U12" s="71">
         <v>22</v>
       </c>
-      <c r="V12" s="78">
+      <c r="V12" s="75">
         <v>22</v>
       </c>
-      <c r="W12" s="76">
+      <c r="W12" s="73">
         <v>17</v>
       </c>
-      <c r="X12" s="48">
+      <c r="X12" s="47">
         <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A13" s="49">
+      <c r="A13" s="48">
         <v>8</v>
       </c>
-      <c r="B13" s="49">
+      <c r="B13" s="48">
         <f t="shared" si="11"/>
         <v>1.4000000000000004</v>
       </c>
-      <c r="C13" s="65">
+      <c r="C13" s="64">
         <v>4</v>
       </c>
-      <c r="D13" s="48">
+      <c r="D13" s="47">
         <f t="shared" si="2"/>
         <v>128</v>
       </c>
-      <c r="E13" s="48">
+      <c r="E13" s="47">
         <f t="shared" si="3"/>
         <v>52.389056098930652</v>
       </c>
-      <c r="F13" s="48">
+      <c r="F13" s="47">
         <f t="shared" si="4"/>
         <v>3143.3433659358393</v>
       </c>
-      <c r="G13" s="48">
+      <c r="G13" s="47">
         <f t="shared" si="5"/>
         <v>88.206332105316818</v>
       </c>
-      <c r="H13" s="48">
+      <c r="H13" s="47">
         <f t="shared" si="6"/>
         <v>40</v>
       </c>
@@ -4249,77 +4256,77 @@
       <c r="L13" s="1">
         <v>8</v>
       </c>
-      <c r="M13" s="77">
+      <c r="M13" s="74">
         <f t="shared" si="7"/>
         <v>3428.5714285714284</v>
       </c>
-      <c r="N13" s="74">
+      <c r="N13" s="71">
         <f t="shared" si="8"/>
         <v>3120</v>
       </c>
-      <c r="O13" s="80">
+      <c r="O13" s="77">
         <f t="shared" si="9"/>
         <v>2512</v>
       </c>
-      <c r="P13" s="76">
+      <c r="P13" s="73">
         <f t="shared" si="0"/>
         <v>1740.25</v>
       </c>
-      <c r="Q13" s="48">
+      <c r="Q13" s="47">
         <f t="shared" si="1"/>
         <v>2056</v>
       </c>
-      <c r="R13" s="64">
+      <c r="R13" s="63">
         <f t="shared" si="10"/>
         <v>22.051583026329205</v>
       </c>
       <c r="S13" s="1">
         <v>8</v>
       </c>
-      <c r="T13" s="77">
+      <c r="T13" s="74">
         <v>32</v>
       </c>
-      <c r="U13" s="74">
+      <c r="U13" s="71">
         <v>25</v>
       </c>
-      <c r="V13" s="78">
+      <c r="V13" s="75">
         <v>25</v>
       </c>
-      <c r="W13" s="76">
+      <c r="W13" s="73">
         <v>19</v>
       </c>
-      <c r="X13" s="48">
+      <c r="X13" s="47">
         <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A14" s="49">
+      <c r="A14" s="48">
         <v>9</v>
       </c>
-      <c r="B14" s="49">
+      <c r="B14" s="48">
         <f t="shared" si="11"/>
         <v>1.4500000000000004</v>
       </c>
-      <c r="C14" s="65">
+      <c r="C14" s="64">
         <v>5</v>
       </c>
-      <c r="D14" s="48">
+      <c r="D14" s="47">
         <f t="shared" si="2"/>
         <v>134</v>
       </c>
-      <c r="E14" s="48">
+      <c r="E14" s="47">
         <f t="shared" si="3"/>
         <v>59.487735836358524</v>
       </c>
-      <c r="F14" s="48">
+      <c r="F14" s="47">
         <f t="shared" si="4"/>
         <v>3569.2641501815115</v>
       </c>
-      <c r="G14" s="48">
+      <c r="G14" s="47">
         <f t="shared" si="5"/>
         <v>86.518310929661936</v>
       </c>
-      <c r="H14" s="48">
+      <c r="H14" s="47">
         <f t="shared" si="6"/>
         <v>49.5</v>
       </c>
@@ -4328,77 +4335,77 @@
       <c r="L14" s="1">
         <v>9</v>
       </c>
-      <c r="M14" s="77">
+      <c r="M14" s="74">
         <f t="shared" si="7"/>
         <v>4291.5714285714284</v>
       </c>
-      <c r="N14" s="74">
+      <c r="N14" s="71">
         <f t="shared" si="8"/>
         <v>3690</v>
       </c>
-      <c r="O14" s="80">
+      <c r="O14" s="77">
         <f t="shared" si="9"/>
         <v>2979</v>
       </c>
-      <c r="P14" s="76">
+      <c r="P14" s="73">
         <f t="shared" si="0"/>
         <v>2600</v>
       </c>
-      <c r="Q14" s="48">
+      <c r="Q14" s="47">
         <f t="shared" si="1"/>
         <v>2364.5</v>
       </c>
-      <c r="R14" s="64">
+      <c r="R14" s="63">
         <f t="shared" si="10"/>
         <v>24.22512706030534</v>
       </c>
       <c r="S14" s="1">
         <v>9</v>
       </c>
-      <c r="T14" s="77">
+      <c r="T14" s="74">
         <v>36</v>
       </c>
-      <c r="U14" s="74">
+      <c r="U14" s="71">
         <v>28</v>
       </c>
-      <c r="V14" s="78">
+      <c r="V14" s="75">
         <v>28</v>
       </c>
-      <c r="W14" s="76">
+      <c r="W14" s="73">
         <v>21</v>
       </c>
-      <c r="X14" s="48">
+      <c r="X14" s="47">
         <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A15" s="49">
+      <c r="A15" s="48">
         <v>10</v>
       </c>
-      <c r="B15" s="49">
+      <c r="B15" s="48">
         <f t="shared" si="11"/>
         <v>1.5000000000000004</v>
       </c>
-      <c r="C15" s="65">
+      <c r="C15" s="64">
         <v>6</v>
       </c>
-      <c r="D15" s="48">
+      <c r="D15" s="47">
         <f t="shared" si="2"/>
         <v>140</v>
       </c>
-      <c r="E15" s="48">
+      <c r="E15" s="47">
         <f t="shared" si="3"/>
         <v>67.182493960703468</v>
       </c>
-      <c r="F15" s="48">
+      <c r="F15" s="47">
         <f t="shared" si="4"/>
         <v>4030.949637642208</v>
       </c>
-      <c r="G15" s="48">
+      <c r="G15" s="47">
         <f t="shared" si="5"/>
         <v>84.705509949529969</v>
       </c>
-      <c r="H15" s="48">
+      <c r="H15" s="47">
         <f t="shared" si="6"/>
         <v>60</v>
       </c>
@@ -4407,71 +4414,71 @@
       <c r="L15" s="1">
         <v>10</v>
       </c>
-      <c r="M15" s="77">
+      <c r="M15" s="74">
         <f t="shared" si="7"/>
         <v>5362.2857142857138</v>
       </c>
-      <c r="N15" s="74">
+      <c r="N15" s="71">
         <f t="shared" si="8"/>
         <v>4320</v>
       </c>
-      <c r="O15" s="80">
+      <c r="O15" s="77">
         <f t="shared" si="9"/>
         <v>3500</v>
       </c>
-      <c r="P15" s="76">
+      <c r="P15" s="73">
         <f t="shared" si="0"/>
         <v>3760.25</v>
       </c>
-      <c r="Q15" s="48">
+      <c r="Q15" s="47">
         <f t="shared" si="1"/>
         <v>2700</v>
       </c>
-      <c r="R15" s="64">
+      <c r="R15" s="63">
         <f t="shared" si="10"/>
         <v>26.258708084354289</v>
       </c>
       <c r="S15" s="1">
         <v>10</v>
       </c>
-      <c r="T15" s="77">
+      <c r="T15" s="74">
         <v>40</v>
       </c>
-      <c r="U15" s="74">
+      <c r="U15" s="71">
         <v>31</v>
       </c>
-      <c r="V15" s="78">
+      <c r="V15" s="75">
         <v>31</v>
       </c>
-      <c r="W15" s="76">
+      <c r="W15" s="73">
         <v>23</v>
       </c>
-      <c r="X15" s="48">
+      <c r="X15" s="47">
         <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A16" s="49">
+      <c r="A16" s="48">
         <v>11</v>
       </c>
-      <c r="B16" s="49">
+      <c r="B16" s="48">
         <f>B15+0.15</f>
         <v>1.6500000000000004</v>
       </c>
-      <c r="C16" s="68"/>
-      <c r="D16" s="48">
+      <c r="C16" s="67"/>
+      <c r="D16" s="47">
         <f t="shared" si="2"/>
         <v>146</v>
       </c>
-      <c r="E16" s="48">
+      <c r="E16" s="47">
         <f t="shared" si="3"/>
         <v>75.642631884188177</v>
       </c>
-      <c r="F16" s="48">
+      <c r="F16" s="47">
         <f t="shared" si="4"/>
         <v>4538.5579130512906</v>
       </c>
-      <c r="G16" s="48">
+      <c r="G16" s="47">
         <f t="shared" si="5"/>
         <v>82.745299048063671</v>
       </c>
@@ -4481,20 +4488,20 @@
         <v>11</v>
       </c>
       <c r="M16" s="1"/>
-      <c r="N16" s="74">
+      <c r="N16" s="71">
         <f t="shared" si="8"/>
         <v>5016</v>
       </c>
-      <c r="O16" s="80">
+      <c r="O16" s="77">
         <f t="shared" si="9"/>
         <v>4081</v>
       </c>
       <c r="P16" s="1"/>
-      <c r="Q16" s="48">
+      <c r="Q16" s="47">
         <f t="shared" si="1"/>
         <v>3065.5</v>
       </c>
-      <c r="R16" s="64">
+      <c r="R16" s="63">
         <f t="shared" si="10"/>
         <v>28.133401676341649</v>
       </c>
@@ -4502,39 +4509,39 @@
         <v>11</v>
       </c>
       <c r="T16" s="1"/>
-      <c r="U16" s="74">
+      <c r="U16" s="71">
         <v>34</v>
       </c>
-      <c r="V16" s="78">
+      <c r="V16" s="75">
         <v>34</v>
       </c>
       <c r="W16" s="1"/>
-      <c r="X16" s="48">
+      <c r="X16" s="47">
         <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A17" s="49">
+      <c r="A17" s="48">
         <v>12</v>
       </c>
-      <c r="B17" s="49">
+      <c r="B17" s="48">
         <f>B16+0.15</f>
         <v>1.8000000000000003</v>
       </c>
-      <c r="C17" s="68"/>
-      <c r="D17" s="48">
+      <c r="C17" s="67"/>
+      <c r="D17" s="47">
         <f t="shared" si="2"/>
         <v>152</v>
       </c>
-      <c r="E17" s="48">
+      <c r="E17" s="47">
         <f t="shared" si="3"/>
         <v>85.085536923187675</v>
       </c>
-      <c r="F17" s="48">
+      <c r="F17" s="47">
         <f t="shared" si="4"/>
         <v>5105.1322153912606</v>
       </c>
-      <c r="G17" s="48">
+      <c r="G17" s="47">
         <f t="shared" si="5"/>
         <v>80.610943901069348</v>
       </c>
@@ -4544,20 +4551,20 @@
         <v>12</v>
       </c>
       <c r="M17" s="1"/>
-      <c r="N17" s="74">
+      <c r="N17" s="71">
         <f t="shared" si="8"/>
         <v>5784</v>
       </c>
-      <c r="O17" s="80">
+      <c r="O17" s="77">
         <f t="shared" si="9"/>
         <v>4728</v>
       </c>
       <c r="P17" s="1"/>
-      <c r="Q17" s="48">
+      <c r="Q17" s="47">
         <f t="shared" si="1"/>
         <v>3464</v>
       </c>
-      <c r="R17" s="64">
+      <c r="R17" s="63">
         <f t="shared" si="10"/>
         <v>29.826049243395659</v>
       </c>
@@ -4565,39 +4572,39 @@
         <v>12</v>
       </c>
       <c r="T17" s="1"/>
-      <c r="U17" s="74">
+      <c r="U17" s="71">
         <v>37</v>
       </c>
-      <c r="V17" s="78">
+      <c r="V17" s="75">
         <v>37</v>
       </c>
       <c r="W17" s="1"/>
-      <c r="X17" s="48">
+      <c r="X17" s="47">
         <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A18" s="49">
+      <c r="A18" s="48">
         <v>13</v>
       </c>
-      <c r="B18" s="49">
+      <c r="B18" s="48">
         <f t="shared" ref="B18:B25" si="12">B17+0.15</f>
         <v>1.9500000000000002</v>
       </c>
-      <c r="C18" s="68"/>
-      <c r="D18" s="48">
+      <c r="C18" s="67"/>
+      <c r="D18" s="47">
         <f t="shared" si="2"/>
         <v>158</v>
       </c>
-      <c r="E18" s="48">
+      <c r="E18" s="47">
         <f t="shared" si="3"/>
         <v>95.790339917193066</v>
       </c>
-      <c r="F18" s="48">
+      <c r="F18" s="47">
         <f t="shared" si="4"/>
         <v>5747.4203950315841</v>
       </c>
-      <c r="G18" s="48">
+      <c r="G18" s="47">
         <f t="shared" si="5"/>
         <v>78.270861636279875</v>
       </c>
@@ -4607,20 +4614,20 @@
         <v>13</v>
       </c>
       <c r="M18" s="1"/>
-      <c r="N18" s="74">
+      <c r="N18" s="71">
         <f t="shared" si="8"/>
         <v>6630</v>
       </c>
-      <c r="O18" s="80">
+      <c r="O18" s="77">
         <f t="shared" si="9"/>
         <v>5447</v>
       </c>
       <c r="P18" s="1"/>
-      <c r="Q18" s="48">
+      <c r="Q18" s="47">
         <f t="shared" si="1"/>
         <v>3898.5</v>
       </c>
-      <c r="R18" s="64">
+      <c r="R18" s="63">
         <f t="shared" si="10"/>
         <v>31.308344654511949</v>
       </c>
@@ -4628,39 +4635,39 @@
         <v>13</v>
       </c>
       <c r="T18" s="1"/>
-      <c r="U18" s="74">
+      <c r="U18" s="71">
         <v>40</v>
       </c>
-      <c r="V18" s="78">
+      <c r="V18" s="75">
         <v>40</v>
       </c>
       <c r="W18" s="1"/>
-      <c r="X18" s="48">
+      <c r="X18" s="47">
         <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A19" s="49">
+      <c r="A19" s="48">
         <v>14</v>
       </c>
-      <c r="B19" s="49">
+      <c r="B19" s="48">
         <f t="shared" si="12"/>
         <v>2.1</v>
       </c>
-      <c r="C19" s="68"/>
-      <c r="D19" s="48">
+      <c r="C19" s="67"/>
+      <c r="D19" s="47">
         <f t="shared" si="2"/>
         <v>164</v>
       </c>
-      <c r="E19" s="48">
+      <c r="E19" s="47">
         <f t="shared" si="3"/>
         <v>108.11545195869232</v>
       </c>
-      <c r="F19" s="48">
+      <c r="F19" s="47">
         <f t="shared" si="4"/>
         <v>6486.927117521539</v>
       </c>
-      <c r="G19" s="48">
+      <c r="G19" s="47">
         <f t="shared" si="5"/>
         <v>75.687741498674228</v>
       </c>
@@ -4670,20 +4677,20 @@
         <v>14</v>
       </c>
       <c r="M19" s="1"/>
-      <c r="N19" s="74">
+      <c r="N19" s="71">
         <f t="shared" si="8"/>
         <v>7560</v>
       </c>
-      <c r="O19" s="80">
+      <c r="O19" s="77">
         <f t="shared" si="9"/>
         <v>6244</v>
       </c>
       <c r="P19" s="1"/>
-      <c r="Q19" s="48">
+      <c r="Q19" s="47">
         <f t="shared" si="1"/>
         <v>4372</v>
       </c>
-      <c r="R19" s="64">
+      <c r="R19" s="63">
         <f t="shared" si="10"/>
         <v>32.545728844429917</v>
       </c>
@@ -4691,39 +4698,39 @@
         <v>14</v>
       </c>
       <c r="T19" s="1"/>
-      <c r="U19" s="74">
+      <c r="U19" s="71">
         <v>43</v>
       </c>
-      <c r="V19" s="78">
+      <c r="V19" s="75">
         <v>43</v>
       </c>
       <c r="W19" s="1"/>
-      <c r="X19" s="48">
+      <c r="X19" s="47">
         <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A20" s="49">
+      <c r="A20" s="48">
         <v>15</v>
       </c>
-      <c r="B20" s="49">
+      <c r="B20" s="48">
         <f t="shared" si="12"/>
         <v>2.25</v>
       </c>
-      <c r="C20" s="68"/>
-      <c r="D20" s="48">
+      <c r="C20" s="67"/>
+      <c r="D20" s="47">
         <f t="shared" si="2"/>
         <v>170</v>
       </c>
-      <c r="E20" s="48">
+      <c r="E20" s="47">
         <f t="shared" si="3"/>
         <v>122.52108200006279</v>
       </c>
-      <c r="F20" s="48">
+      <c r="F20" s="47">
         <f t="shared" si="4"/>
         <v>7351.2649200037677</v>
       </c>
-      <c r="G20" s="48">
+      <c r="G20" s="47">
         <f t="shared" si="5"/>
         <v>72.817506039296532</v>
       </c>
@@ -4733,20 +4740,20 @@
         <v>15</v>
       </c>
       <c r="M20" s="1"/>
-      <c r="N20" s="74">
+      <c r="N20" s="71">
         <f t="shared" si="8"/>
         <v>8580</v>
       </c>
-      <c r="O20" s="80">
+      <c r="O20" s="77">
         <f t="shared" si="9"/>
         <v>7125</v>
       </c>
       <c r="P20" s="1"/>
-      <c r="Q20" s="48">
+      <c r="Q20" s="47">
         <f t="shared" si="1"/>
         <v>4887.5</v>
       </c>
-      <c r="R20" s="64">
+      <c r="R20" s="63">
         <f t="shared" si="10"/>
         <v>33.496052778076404</v>
       </c>
@@ -4754,39 +4761,39 @@
         <v>15</v>
       </c>
       <c r="T20" s="1"/>
-      <c r="U20" s="74">
+      <c r="U20" s="71">
         <v>46</v>
       </c>
-      <c r="V20" s="78">
+      <c r="V20" s="75">
         <v>46</v>
       </c>
       <c r="W20" s="1"/>
-      <c r="X20" s="48">
+      <c r="X20" s="47">
         <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A21" s="49">
+      <c r="A21" s="48">
         <v>16</v>
       </c>
-      <c r="B21" s="49">
+      <c r="B21" s="48">
         <f t="shared" si="12"/>
         <v>2.4</v>
       </c>
-      <c r="C21" s="68"/>
-      <c r="D21" s="48">
+      <c r="C21" s="67"/>
+      <c r="D21" s="47">
         <f t="shared" si="2"/>
         <v>176</v>
       </c>
-      <c r="E21" s="48">
+      <c r="E21" s="47">
         <f t="shared" si="3"/>
         <v>139.59815003314424</v>
       </c>
-      <c r="F21" s="48">
+      <c r="F21" s="47">
         <f t="shared" si="4"/>
         <v>8375.8890019886549</v>
       </c>
-      <c r="G21" s="48">
+      <c r="G21" s="47">
         <f t="shared" si="5"/>
         <v>69.608083904850105</v>
       </c>
@@ -4794,20 +4801,20 @@
         <v>16</v>
       </c>
       <c r="M21" s="1"/>
-      <c r="N21" s="74">
+      <c r="N21" s="71">
         <f t="shared" si="8"/>
         <v>9696</v>
       </c>
-      <c r="O21" s="80">
+      <c r="O21" s="77">
         <f t="shared" si="9"/>
         <v>8096</v>
       </c>
       <c r="P21" s="1"/>
-      <c r="Q21" s="48">
+      <c r="Q21" s="47">
         <f t="shared" si="1"/>
         <v>5448</v>
       </c>
-      <c r="R21" s="64">
+      <c r="R21" s="63">
         <f t="shared" si="10"/>
         <v>34.107961113376547</v>
       </c>
@@ -4815,39 +4822,39 @@
         <v>16</v>
       </c>
       <c r="T21" s="1"/>
-      <c r="U21" s="74">
+      <c r="U21" s="71">
         <v>49</v>
       </c>
-      <c r="V21" s="78">
+      <c r="V21" s="75">
         <v>49</v>
       </c>
       <c r="W21" s="1"/>
-      <c r="X21" s="48">
+      <c r="X21" s="47">
         <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A22" s="49">
+      <c r="A22" s="48">
         <v>17</v>
       </c>
-      <c r="B22" s="49">
+      <c r="B22" s="48">
         <f t="shared" si="12"/>
         <v>2.5499999999999998</v>
       </c>
-      <c r="C22" s="68"/>
-      <c r="D22" s="48">
+      <c r="C22" s="67"/>
+      <c r="D22" s="47">
         <f t="shared" si="2"/>
         <v>182</v>
       </c>
-      <c r="E22" s="48">
+      <c r="E22" s="47">
         <f t="shared" si="3"/>
         <v>160.10541234668784</v>
       </c>
-      <c r="F22" s="48">
+      <c r="F22" s="47">
         <f t="shared" si="4"/>
         <v>9606.3247408012703</v>
       </c>
-      <c r="G22" s="48">
+      <c r="G22" s="47">
         <f t="shared" si="5"/>
         <v>65.997960059905978</v>
       </c>
@@ -4855,20 +4862,20 @@
         <v>17</v>
       </c>
       <c r="M22" s="1"/>
-      <c r="N22" s="74">
+      <c r="N22" s="71">
         <f t="shared" si="8"/>
         <v>10914</v>
       </c>
-      <c r="O22" s="80">
+      <c r="O22" s="77">
         <f t="shared" si="9"/>
         <v>9163</v>
       </c>
       <c r="P22" s="1"/>
-      <c r="Q22" s="48">
+      <c r="Q22" s="47">
         <f t="shared" si="1"/>
         <v>6056.5</v>
       </c>
-      <c r="R22" s="64">
+      <c r="R22" s="63">
         <f t="shared" si="10"/>
         <v>34.318939231151106</v>
       </c>
@@ -4876,39 +4883,39 @@
         <v>17</v>
       </c>
       <c r="T22" s="1"/>
-      <c r="U22" s="74">
+      <c r="U22" s="71">
         <v>52</v>
       </c>
-      <c r="V22" s="78">
+      <c r="V22" s="75">
         <v>52</v>
       </c>
       <c r="W22" s="1"/>
-      <c r="X22" s="48">
+      <c r="X22" s="47">
         <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A23" s="49">
+      <c r="A23" s="48">
         <v>18</v>
       </c>
-      <c r="B23" s="49">
+      <c r="B23" s="48">
         <f t="shared" si="12"/>
         <v>2.6999999999999997</v>
       </c>
-      <c r="C23" s="68"/>
-      <c r="D23" s="48">
+      <c r="C23" s="67"/>
+      <c r="D23" s="47">
         <f t="shared" si="2"/>
         <v>188</v>
       </c>
-      <c r="E23" s="48">
+      <c r="E23" s="47">
         <f t="shared" si="3"/>
         <v>185.01713130052181</v>
       </c>
-      <c r="F23" s="48">
+      <c r="F23" s="47">
         <f t="shared" si="4"/>
         <v>11101.027878031309</v>
       </c>
-      <c r="G23" s="48">
+      <c r="G23" s="47">
         <f t="shared" si="5"/>
         <v>61.914463076812325</v>
       </c>
@@ -4916,20 +4923,20 @@
         <v>18</v>
       </c>
       <c r="M23" s="1"/>
-      <c r="N23" s="74">
+      <c r="N23" s="71">
         <f t="shared" si="8"/>
         <v>12240</v>
       </c>
-      <c r="O23" s="80">
+      <c r="O23" s="77">
         <f t="shared" si="9"/>
         <v>10332</v>
       </c>
       <c r="P23" s="1"/>
-      <c r="Q23" s="48">
+      <c r="Q23" s="47">
         <f t="shared" si="1"/>
         <v>6716</v>
       </c>
-      <c r="R23" s="64">
+      <c r="R23" s="63">
         <f t="shared" si="10"/>
         <v>34.052954692246779</v>
       </c>
@@ -4937,39 +4944,39 @@
         <v>18</v>
       </c>
       <c r="T23" s="1"/>
-      <c r="U23" s="74">
+      <c r="U23" s="71">
         <v>55</v>
       </c>
-      <c r="V23" s="78">
+      <c r="V23" s="75">
         <v>55</v>
       </c>
       <c r="W23" s="1"/>
-      <c r="X23" s="48">
+      <c r="X23" s="47">
         <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A24" s="49">
+      <c r="A24" s="48">
         <v>19</v>
       </c>
-      <c r="B24" s="49">
+      <c r="B24" s="48">
         <f t="shared" si="12"/>
         <v>2.8499999999999996</v>
       </c>
-      <c r="C24" s="68"/>
-      <c r="D24" s="48">
+      <c r="C24" s="67"/>
+      <c r="D24" s="47">
         <f t="shared" si="2"/>
         <v>194</v>
       </c>
-      <c r="E24" s="48">
+      <c r="E24" s="47">
         <f t="shared" si="3"/>
         <v>215.58428452718766</v>
       </c>
-      <c r="F24" s="48">
+      <c r="F24" s="47">
         <f t="shared" si="4"/>
         <v>12935.05707163126</v>
       </c>
-      <c r="G24" s="48">
+      <c r="G24" s="47">
         <f t="shared" si="5"/>
         <v>57.271741807794839</v>
       </c>
@@ -4977,20 +4984,20 @@
         <v>19</v>
       </c>
       <c r="M24" s="1"/>
-      <c r="N24" s="74">
+      <c r="N24" s="71">
         <f t="shared" si="8"/>
         <v>13680</v>
       </c>
-      <c r="O24" s="80">
+      <c r="O24" s="77">
         <f t="shared" si="9"/>
         <v>11609</v>
       </c>
       <c r="P24" s="1"/>
-      <c r="Q24" s="48">
+      <c r="Q24" s="47">
         <f t="shared" si="1"/>
         <v>7429.5</v>
       </c>
-      <c r="R24" s="64">
+      <c r="R24" s="63">
         <f t="shared" si="10"/>
         <v>33.217610248521005</v>
       </c>
@@ -4998,39 +5005,39 @@
         <v>19</v>
       </c>
       <c r="T24" s="1"/>
-      <c r="U24" s="74">
+      <c r="U24" s="71">
         <v>58</v>
       </c>
-      <c r="V24" s="78">
+      <c r="V24" s="75">
         <v>58</v>
       </c>
       <c r="W24" s="1"/>
-      <c r="X24" s="48">
+      <c r="X24" s="47">
         <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A25" s="49">
+      <c r="A25" s="48">
         <v>20</v>
       </c>
-      <c r="B25" s="49">
+      <c r="B25" s="48">
         <f t="shared" si="12"/>
         <v>2.9999999999999996</v>
       </c>
-      <c r="C25" s="68"/>
-      <c r="D25" s="48">
+      <c r="C25" s="67"/>
+      <c r="D25" s="47">
         <f t="shared" si="2"/>
         <v>200</v>
       </c>
-      <c r="E25" s="48">
+      <c r="E25" s="47">
         <f t="shared" si="3"/>
         <v>253.4131591025766</v>
       </c>
-      <c r="F25" s="48">
+      <c r="F25" s="47">
         <f t="shared" si="4"/>
         <v>15204.789546154596</v>
       </c>
-      <c r="G25" s="48">
+      <c r="G25" s="47">
         <f t="shared" si="5"/>
         <v>51.968375105473854</v>
       </c>
@@ -5038,20 +5045,20 @@
         <v>20</v>
       </c>
       <c r="M25" s="1"/>
-      <c r="N25" s="74">
+      <c r="N25" s="71">
         <f t="shared" si="8"/>
         <v>15240</v>
       </c>
-      <c r="O25" s="80">
+      <c r="O25" s="77">
         <f t="shared" si="9"/>
         <v>13000</v>
       </c>
       <c r="P25" s="1"/>
-      <c r="Q25" s="48">
+      <c r="Q25" s="47">
         <f t="shared" si="1"/>
         <v>8200</v>
       </c>
-      <c r="R25" s="64">
+      <c r="R25" s="63">
         <f t="shared" si="10"/>
         <v>31.700708814339052</v>
       </c>
@@ -5059,14 +5066,14 @@
         <v>20</v>
       </c>
       <c r="T25" s="1"/>
-      <c r="U25" s="74">
+      <c r="U25" s="71">
         <v>61</v>
       </c>
-      <c r="V25" s="78">
+      <c r="V25" s="75">
         <v>61</v>
       </c>
       <c r="W25" s="1"/>
-      <c r="X25" s="48">
+      <c r="X25" s="47">
         <v>106</v>
       </c>
     </row>
@@ -5074,11 +5081,11 @@
       <c r="L26" s="1">
         <v>21</v>
       </c>
-      <c r="O26" s="73"/>
+      <c r="O26" s="70"/>
       <c r="S26" s="1">
         <v>21</v>
       </c>
-      <c r="V26" s="73"/>
+      <c r="V26" s="70"/>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="L27" s="1">
@@ -5089,7 +5096,7 @@
       </c>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="R28" s="64"/>
+      <c r="R28" s="63"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>